<commit_message>
Update CatSim material calculator.xlsx
</commit_message>
<xml_diff>
--- a/tools/CatSim material calculator.xlsx
+++ b/tools/CatSim material calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\200003237\Documents\Projects\XCIST\XCIST from Paul's old laptop\Materials\New materials for XCIST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\200003237\Documents\GitHub\documentation\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B9D4D2-C9EA-4658-9B74-9200D56FE2C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431A4BB9-4175-4B36-B152-6DF49CC53CB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" activeTab="1" xr2:uid="{B8F9F76C-33C1-418E-8852-058650A875FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{B8F9F76C-33C1-418E-8852-058650A875FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="425">
   <si>
     <t>element</t>
   </si>
@@ -1945,7 +1945,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2069,6 +2069,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2088,90 +2097,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2183,6 +2108,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2234,10 +2168,103 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2255,9 +2282,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2270,16 +2294,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2300,22 +2318,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2643,10 +2647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8CB8E5-6694-4F1B-B671-195116FAC06A}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2677,52 +2681,60 @@
       <c r="L1" s="31"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
     </row>
     <row r="3" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="60" t="s">
         <v>390</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+    </row>
+    <row r="4" spans="1:12" s="54" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="136" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="136"/>
+      <c r="C4" s="136"/>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="57" t="s">
         <v>391</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="57" t="s">
         <v>419</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-    </row>
-    <row r="7" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+    </row>
+    <row r="8" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="62" t="s">
         <v>420</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A7:C7"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2734,8 +2746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE334929-57FE-4A9D-B51A-4CE49032E816}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2751,107 +2763,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="93" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="66"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="95"/>
       <c r="O1" s="28" t="s">
         <v>257</v>
       </c>
       <c r="P1" s="48"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="68" t="s">
         <v>385</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
       <c r="O2" s="11" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="68" t="s">
         <v>413</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="62"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="89"/>
       <c r="O3" s="12" t="str">
         <f>CONCATENATE("# Made with ",Instructions!A$1, " ",Instructions!B$1, ".")</f>
         <v># Made with CatSim material calculator, version 1.0.</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="68" t="s">
         <v>414</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="62"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="89"/>
       <c r="O4" s="23" t="str">
         <f>IF(O12&lt;&gt;"1", CONCATENATE("# Molecular weights from ", Data!$I$1, "."), "")</f>
         <v># Molecular weights from https://www.nist.gov/pml/atomic-weights-and-isotopic-compositions-relative-atomic-masses.</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="69" t="s">
         <v>415</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="131">
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="56">
         <v>1.0045999999999999</v>
       </c>
       <c r="M5" s="10" t="s">
@@ -2864,69 +2876,69 @@
       </c>
     </row>
     <row r="6" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="69" t="s">
         <v>384</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="134" t="s">
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="90" t="s">
         <v>421</v>
       </c>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="132"/>
-      <c r="J6" s="132"/>
-      <c r="K6" s="132"/>
-      <c r="L6" s="132"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="133"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="92"/>
       <c r="O6" s="23" t="str">
         <f>IF($O$12="1", IF(ISBLANK($F$8), "", #N/A), IF(ISBLANK($F$8), "# Material composition source not specified.", CONCATENATE("# Material composition source: ",$F$8)))</f>
         <v># Material composition source: same as density</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="69" t="s">
         <v>380</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="103" t="s">
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="81" t="s">
         <v>422</v>
       </c>
-      <c r="H7" s="104"/>
-      <c r="I7" s="104"/>
-      <c r="J7" s="104"/>
-      <c r="K7" s="104"/>
-      <c r="L7" s="104"/>
-      <c r="M7" s="104"/>
-      <c r="N7" s="104"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
       <c r="O7" s="24"/>
     </row>
     <row r="8" spans="1:16" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="69" t="s">
         <v>381</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="105" t="s">
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="83" t="s">
         <v>383</v>
       </c>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="106"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="107"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="84"/>
+      <c r="M8" s="84"/>
+      <c r="N8" s="85"/>
       <c r="O8" s="23" t="str">
         <f>IF($O$12="1","# Elemental material: ", "# Material name:")</f>
         <v># Material name:</v>
@@ -2941,69 +2953,69 @@
       <c r="D9" s="49">
         <v>6</v>
       </c>
-      <c r="E9" s="73" t="s">
+      <c r="E9" s="102" t="s">
         <v>402</v>
       </c>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="74"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="70"/>
       <c r="O9" s="23" t="str">
         <f>IF($O$12="1", IF(ISBLANK($G$7),_xlfn.CONCAT("# ",$A$18, " (", $C$18,")"), _xlfn.CONCAT("# ", $G$7)), IF(ISBLANK($G$7),"# not specified", _xlfn.CONCAT("# ", $G$7)))</f>
         <v># nomal saline (9% NaCl in water)</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="68" t="s">
         <v>382</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="61"/>
-      <c r="N10" s="61"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
       <c r="O10" s="24"/>
     </row>
     <row r="11" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="69" t="s">
         <v>266</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
       <c r="O11" s="24" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="71" t="s">
         <v>404</v>
       </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="83" t="s">
+      <c r="B12" s="72"/>
+      <c r="C12" s="111" t="s">
         <v>256</v>
       </c>
       <c r="D12" s="86" t="s">
@@ -3015,69 +3027,69 @@
       <c r="F12" s="86" t="s">
         <v>396</v>
       </c>
-      <c r="G12" s="75"/>
+      <c r="G12" s="103"/>
       <c r="H12" s="86" t="s">
         <v>397</v>
       </c>
       <c r="I12" s="86" t="s">
         <v>392</v>
       </c>
-      <c r="J12" s="78"/>
-      <c r="K12" s="97" t="s">
+      <c r="J12" s="106"/>
+      <c r="K12" s="75" t="s">
         <v>263</v>
       </c>
-      <c r="L12" s="98"/>
-      <c r="M12" s="101" t="s">
+      <c r="L12" s="76"/>
+      <c r="M12" s="79" t="s">
         <v>262</v>
       </c>
-      <c r="N12" s="97"/>
+      <c r="N12" s="75"/>
       <c r="O12" s="23" t="str">
         <f>IF(COUNTA(A18:A29)&lt;&gt;COUNTA(B18:B29),"Error! Different number of entries for Symbol and Number of atoms per molecule.", _xlfn.VALUETOTEXT(COUNTA(B18:B29)))</f>
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="95"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="84"/>
+      <c r="A13" s="73"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="112"/>
       <c r="D13" s="87"/>
       <c r="E13" s="87"/>
       <c r="F13" s="87"/>
-      <c r="G13" s="76"/>
+      <c r="G13" s="104"/>
       <c r="H13" s="87"/>
       <c r="I13" s="87"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="99"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="99"/>
+      <c r="J13" s="107"/>
+      <c r="K13" s="77"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="80"/>
+      <c r="N13" s="77"/>
       <c r="O13" s="24"/>
     </row>
     <row r="14" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="109" t="s">
         <v>264</v>
       </c>
-      <c r="B14" s="89" t="s">
+      <c r="B14" s="64" t="s">
         <v>411</v>
       </c>
-      <c r="C14" s="84"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="87"/>
       <c r="E14" s="87"/>
       <c r="F14" s="87"/>
-      <c r="G14" s="76"/>
+      <c r="G14" s="104"/>
       <c r="H14" s="87"/>
       <c r="I14" s="87"/>
-      <c r="J14" s="79"/>
-      <c r="K14" s="67" t="s">
+      <c r="J14" s="107"/>
+      <c r="K14" s="96" t="s">
         <v>260</v>
       </c>
-      <c r="L14" s="69" t="s">
+      <c r="L14" s="98" t="s">
         <v>392</v>
       </c>
-      <c r="M14" s="71" t="s">
+      <c r="M14" s="100" t="s">
         <v>260</v>
       </c>
-      <c r="N14" s="67" t="s">
+      <c r="N14" s="96" t="s">
         <v>392</v>
       </c>
       <c r="O14" s="24" t="str">
@@ -3086,57 +3098,57 @@
       </c>
     </row>
     <row r="15" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="81"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="84"/>
+      <c r="A15" s="109"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="112"/>
       <c r="D15" s="87"/>
       <c r="E15" s="87"/>
       <c r="F15" s="87"/>
-      <c r="G15" s="76"/>
+      <c r="G15" s="104"/>
       <c r="H15" s="87"/>
       <c r="I15" s="87"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="71"/>
-      <c r="N15" s="67"/>
+      <c r="J15" s="107"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="100"/>
+      <c r="N15" s="96"/>
       <c r="O15" s="24" t="str">
         <f>IF($O$12="1", IF(ISBLANK($L$5),FIXED(_xlfn.XLOOKUP($A18,Data!$T$6:$T$123,Data!$V$6:$V$123,#N/A),$D$9),FIXED($L$5,$D$9)),IF(ISBLANK($L$5),"Error! Density value not specified!",FIXED($L$5,$D$9)))</f>
         <v>1.004600</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="81"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="84"/>
+      <c r="A16" s="109"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="112"/>
       <c r="D16" s="87"/>
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
-      <c r="G16" s="76"/>
+      <c r="G16" s="104"/>
       <c r="H16" s="87"/>
       <c r="I16" s="87"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="71"/>
-      <c r="N16" s="67"/>
+      <c r="J16" s="107"/>
+      <c r="K16" s="96"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="100"/>
+      <c r="N16" s="96"/>
       <c r="O16" s="24"/>
     </row>
     <row r="17" spans="1:15" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="82"/>
-      <c r="B17" s="90"/>
-      <c r="C17" s="85"/>
+      <c r="A17" s="110"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="113"/>
       <c r="D17" s="88"/>
       <c r="E17" s="88"/>
       <c r="F17" s="88"/>
-      <c r="G17" s="76"/>
+      <c r="G17" s="104"/>
       <c r="H17" s="88"/>
       <c r="I17" s="88"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="70"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="68"/>
+      <c r="J17" s="107"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="99"/>
+      <c r="M17" s="101"/>
+      <c r="N17" s="97"/>
       <c r="O17" s="24" t="s">
         <v>389</v>
       </c>
@@ -3164,7 +3176,7 @@
         <f>IF(ISBLANK($A18), "", B18*E18)</f>
         <v>72342.365750000012</v>
       </c>
-      <c r="G18" s="76"/>
+      <c r="G18" s="104"/>
       <c r="H18" s="6">
         <f>D18</f>
         <v>1</v>
@@ -3173,7 +3185,7 @@
         <f>IF(ISBLANK($B18), "", F18/F$33)</f>
         <v>0.11089927566762281</v>
       </c>
-      <c r="J18" s="79"/>
+      <c r="J18" s="107"/>
       <c r="K18" s="14" cm="1">
         <f t="array" ref="K18:L21">_xlfn._xlws.SORT(H18:INDEX(H18:I29,O12,2),1,1,FALSE)</f>
         <v>1</v>
@@ -3217,7 +3229,7 @@
         <f>IF(ISBLANK($A19), "", B19*E19)</f>
         <v>574138.46900000004</v>
       </c>
-      <c r="G19" s="76"/>
+      <c r="G19" s="104"/>
       <c r="H19" s="6">
         <f t="shared" ref="H19:H29" si="0">D19</f>
         <v>8</v>
@@ -3226,7 +3238,7 @@
         <f>IF(ISBLANK($B19), "", F19/F$33)</f>
         <v>0.88014180466607017</v>
       </c>
-      <c r="J19" s="79"/>
+      <c r="J19" s="107"/>
       <c r="K19" s="14">
         <v>8</v>
       </c>
@@ -3269,7 +3281,7 @@
         <f>IF(ISBLANK($A20), "", B20*E20)</f>
         <v>2298.976928</v>
       </c>
-      <c r="G20" s="76"/>
+      <c r="G20" s="104"/>
       <c r="H20" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3278,7 +3290,7 @@
         <f>IF(ISBLANK($B20), "", F20/F$33)</f>
         <v>3.5242817047599329E-3</v>
       </c>
-      <c r="J20" s="79"/>
+      <c r="J20" s="107"/>
       <c r="K20" s="14">
         <v>11</v>
       </c>
@@ -3321,7 +3333,7 @@
         <f>IF(ISBLANK($A21), "", B21*E21)</f>
         <v>3545.1499999999996</v>
       </c>
-      <c r="G21" s="76"/>
+      <c r="G21" s="104"/>
       <c r="H21" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3330,7 +3342,7 @@
         <f>IF(ISBLANK($B21), "", F21/F$33)</f>
         <v>5.4346379615470746E-3</v>
       </c>
-      <c r="J21" s="79"/>
+      <c r="J21" s="107"/>
       <c r="K21" s="14">
         <v>17</v>
       </c>
@@ -3369,7 +3381,7 @@
         <f t="shared" ref="F22:F29" si="3">IF(ISBLANK($A22), "", B22*E22)</f>
         <v/>
       </c>
-      <c r="G22" s="76"/>
+      <c r="G22" s="104"/>
       <c r="H22" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3378,7 +3390,7 @@
         <f t="shared" ref="I22:I29" si="4">IF(ISBLANK($B22), "", F22/F$33)</f>
         <v/>
       </c>
-      <c r="J22" s="79"/>
+      <c r="J22" s="107"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
       <c r="M22" s="8" t="str">
@@ -3413,7 +3425,7 @@
         <f t="shared" ref="F23:F24" si="5">IF(ISBLANK($A23), "", B23*E23)</f>
         <v/>
       </c>
-      <c r="G23" s="76"/>
+      <c r="G23" s="104"/>
       <c r="H23" s="6" t="str">
         <f t="shared" ref="H23:H24" si="6">D23</f>
         <v/>
@@ -3422,7 +3434,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J23" s="79"/>
+      <c r="J23" s="107"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
       <c r="M23" s="8" t="str">
@@ -3457,7 +3469,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="G24" s="76"/>
+      <c r="G24" s="104"/>
       <c r="H24" s="6" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3466,7 +3478,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J24" s="79"/>
+      <c r="J24" s="107"/>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
       <c r="M24" s="8" t="str">
@@ -3501,7 +3513,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="G25" s="76"/>
+      <c r="G25" s="104"/>
       <c r="H25" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3510,7 +3522,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J25" s="79"/>
+      <c r="J25" s="107"/>
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
       <c r="M25" s="8" t="str">
@@ -3545,7 +3557,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="G26" s="76"/>
+      <c r="G26" s="104"/>
       <c r="H26" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3554,7 +3566,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J26" s="79"/>
+      <c r="J26" s="107"/>
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
       <c r="M26" s="8" t="str">
@@ -3589,7 +3601,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="G27" s="76"/>
+      <c r="G27" s="104"/>
       <c r="H27" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3598,7 +3610,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J27" s="79"/>
+      <c r="J27" s="107"/>
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
       <c r="M27" s="8" t="str">
@@ -3633,7 +3645,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="G28" s="76"/>
+      <c r="G28" s="104"/>
       <c r="H28" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3642,7 +3654,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J28" s="79"/>
+      <c r="J28" s="107"/>
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
       <c r="M28" s="8" t="str">
@@ -3677,7 +3689,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="G29" s="77"/>
+      <c r="G29" s="105"/>
       <c r="H29" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3686,7 +3698,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J29" s="80"/>
+      <c r="J29" s="108"/>
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
       <c r="M29" s="9" t="str">
@@ -3703,18 +3715,18 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="91" t="s">
+      <c r="F30" s="66" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F31" s="92"/>
+      <c r="F31" s="67"/>
       <c r="O31" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F32" s="92"/>
+      <c r="F32" s="67"/>
       <c r="O32" s="24" t="str">
         <f>CONCATENATE("# number of iodine atoms per water molecule = ", B$20)</f>
         <v># number of iodine atoms per water molecule = 100</v>
@@ -3753,6 +3765,22 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="32">
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:N6"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="M14:M17"/>
+    <mergeCell ref="N14:N17"/>
+    <mergeCell ref="A11:N11"/>
+    <mergeCell ref="E9:N9"/>
+    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="G12:G29"/>
+    <mergeCell ref="J12:J29"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A10:N10"/>
+    <mergeCell ref="C12:C17"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="F30:F32"/>
     <mergeCell ref="A2:N2"/>
@@ -3769,22 +3797,6 @@
     <mergeCell ref="F12:F17"/>
     <mergeCell ref="I12:I17"/>
     <mergeCell ref="H12:H17"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:N6"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="K14:K17"/>
-    <mergeCell ref="L14:L17"/>
-    <mergeCell ref="M14:M17"/>
-    <mergeCell ref="N14:N17"/>
-    <mergeCell ref="A11:N11"/>
-    <mergeCell ref="E9:N9"/>
-    <mergeCell ref="A4:N4"/>
-    <mergeCell ref="G12:G29"/>
-    <mergeCell ref="J12:J29"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A10:N10"/>
-    <mergeCell ref="C12:C17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{1ADB471B-66ED-4CF3-B497-F05E82931B84}"/>
@@ -3820,120 +3832,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="119" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
       <c r="Q1" s="28" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="114" t="s">
         <v>405</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
       <c r="Q2" s="11" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="114" t="s">
         <v>413</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
       <c r="Q3" s="12" t="str">
         <f>CONCATENATE("# Made with ",Instructions!A$1, " ",Instructions!B$1, ".")</f>
         <v># Made with CatSim material calculator, version 1.0.</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="69" t="s">
         <v>414</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63"/>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
       <c r="Q4" s="23" t="str">
         <f>IF(Q12&lt;&gt;"1", CONCATENATE("# Molecular weights from ", Data!$I$1, "."), "")</f>
         <v># Molecular weights from https://www.nist.gov/pml/atomic-weights-and-isotopic-compositions-relative-atomic-masses.</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="102" t="s">
         <v>416</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="130"/>
-      <c r="L5" s="108" t="s">
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="128" t="s">
         <v>265</v>
       </c>
-      <c r="M5" s="109"/>
-      <c r="N5" s="109"/>
-      <c r="O5" s="109"/>
-      <c r="P5" s="109"/>
+      <c r="M5" s="129"/>
+      <c r="N5" s="129"/>
+      <c r="O5" s="129"/>
+      <c r="P5" s="129"/>
       <c r="Q5" s="23" t="str">
         <f>IF(AND($Q$12="1",ISBLANK($K$5),ISBLANK($D$6)),CONCATENATE("# Density from ", Data!$S$1, "."), IF(ISBLANK($D$6),"# Density source not specified.",_xlfn.CONCAT("# Density source: ",$D$6)))</f>
         <v># Density source not specified.</v>
@@ -3945,19 +3957,19 @@
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="106"/>
-      <c r="L6" s="106"/>
-      <c r="M6" s="106"/>
-      <c r="N6" s="106"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="84"/>
+      <c r="P6" s="84"/>
       <c r="Q6" s="23" t="str">
         <f>IF(ISBLANK($F$8),IF($Q$12=1,"","# Material composition source not specified."),CONCATENATE("# Material composition source: ",$F$8))</f>
         <v># Material composition source not specified.</v>
@@ -3972,16 +3984,16 @@
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="106"/>
-      <c r="L7" s="106"/>
-      <c r="M7" s="106"/>
-      <c r="N7" s="106"/>
-      <c r="O7" s="106"/>
-      <c r="P7" s="106"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
+      <c r="L7" s="84"/>
+      <c r="M7" s="84"/>
+      <c r="N7" s="84"/>
+      <c r="O7" s="84"/>
+      <c r="P7" s="84"/>
       <c r="Q7" s="24"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3992,17 +4004,17 @@
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="106"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="106"/>
-      <c r="O8" s="106"/>
-      <c r="P8" s="106"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="84"/>
+      <c r="M8" s="84"/>
+      <c r="N8" s="84"/>
+      <c r="O8" s="84"/>
+      <c r="P8" s="84"/>
       <c r="Q8" s="23" t="str">
         <f>IF($Q$12="1","# Elemental material: ", "# Material name:")</f>
         <v># Material name:</v>
@@ -4018,83 +4030,83 @@
       <c r="E9" s="49">
         <v>6</v>
       </c>
-      <c r="F9" s="122" t="s">
+      <c r="F9" s="117" t="s">
         <v>402</v>
       </c>
-      <c r="G9" s="123"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="123"/>
-      <c r="M9" s="123"/>
-      <c r="N9" s="123"/>
-      <c r="O9" s="123"/>
-      <c r="P9" s="123"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="118"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="118"/>
+      <c r="M9" s="118"/>
+      <c r="N9" s="118"/>
+      <c r="O9" s="118"/>
+      <c r="P9" s="118"/>
       <c r="Q9" s="23" t="str">
         <f>IF($Q$12="1", IF(ISBLANK($G$7),_xlfn.CONCAT("# ",$F$18, " (", $C$18,")"), _xlfn.CONCAT("# ", $G$7)), IF(ISBLANK($G$7),"# not specified", _xlfn.CONCAT("# ", $G$7)))</f>
         <v># not specified</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="114" t="s">
         <v>382</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
-      <c r="P10" s="62"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
+      <c r="P10" s="89"/>
       <c r="Q10" s="24"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="102" t="s">
         <v>266</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
+      <c r="O11" s="69"/>
+      <c r="P11" s="69"/>
       <c r="Q11" s="24" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="71" t="s">
         <v>404</v>
       </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="120" t="s">
+      <c r="B12" s="72"/>
+      <c r="C12" s="115" t="s">
         <v>264</v>
       </c>
       <c r="D12" s="86" t="s">
         <v>399</v>
       </c>
-      <c r="E12" s="115" t="s">
+      <c r="E12" s="116" t="s">
         <v>400</v>
       </c>
-      <c r="F12" s="83" t="s">
+      <c r="F12" s="111" t="s">
         <v>256</v>
       </c>
       <c r="G12" s="86" t="s">
@@ -4112,66 +4124,66 @@
       <c r="K12" s="86" t="s">
         <v>394</v>
       </c>
-      <c r="L12" s="78"/>
-      <c r="M12" s="116" t="s">
+      <c r="L12" s="106"/>
+      <c r="M12" s="124" t="s">
         <v>409</v>
       </c>
-      <c r="N12" s="117"/>
-      <c r="O12" s="101" t="s">
+      <c r="N12" s="125"/>
+      <c r="O12" s="79" t="s">
         <v>262</v>
       </c>
-      <c r="P12" s="97"/>
+      <c r="P12" s="75"/>
       <c r="Q12" s="23" t="str">
         <f>IF(COUNTA(A18:A29)&lt;&gt;COUNTA(B18:B29),"Error! Different number of entries for Atomic number and Mass fraction.", _xlfn.VALUETOTEXT(COUNTA(B18:B29)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="95"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="81"/>
+      <c r="A13" s="73"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="109"/>
       <c r="D13" s="87"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="84"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="112"/>
       <c r="G13" s="87"/>
       <c r="H13" s="87"/>
       <c r="I13" s="87"/>
       <c r="J13" s="87"/>
       <c r="K13" s="87"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="118"/>
-      <c r="N13" s="119"/>
-      <c r="O13" s="102"/>
-      <c r="P13" s="99"/>
+      <c r="L13" s="107"/>
+      <c r="M13" s="126"/>
+      <c r="N13" s="127"/>
+      <c r="O13" s="80"/>
+      <c r="P13" s="77"/>
       <c r="Q13" s="24"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="112" t="s">
+      <c r="A14" s="121" t="s">
         <v>260</v>
       </c>
-      <c r="B14" s="115" t="s">
+      <c r="B14" s="116" t="s">
         <v>392</v>
       </c>
-      <c r="C14" s="81"/>
+      <c r="C14" s="109"/>
       <c r="D14" s="87"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="84"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="112"/>
       <c r="G14" s="87"/>
       <c r="H14" s="87"/>
       <c r="I14" s="87"/>
       <c r="J14" s="87"/>
       <c r="K14" s="87"/>
-      <c r="L14" s="79"/>
-      <c r="M14" s="67" t="s">
+      <c r="L14" s="107"/>
+      <c r="M14" s="96" t="s">
         <v>260</v>
       </c>
-      <c r="N14" s="69" t="s">
+      <c r="N14" s="98" t="s">
         <v>392</v>
       </c>
-      <c r="O14" s="71" t="s">
+      <c r="O14" s="100" t="s">
         <v>260</v>
       </c>
-      <c r="P14" s="67" t="s">
+      <c r="P14" s="96" t="s">
         <v>392</v>
       </c>
       <c r="Q14" s="24" t="str">
@@ -4180,63 +4192,63 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="113"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="81"/>
+      <c r="A15" s="122"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="109"/>
       <c r="D15" s="87"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="84"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="112"/>
       <c r="G15" s="87"/>
       <c r="H15" s="87"/>
       <c r="I15" s="87"/>
       <c r="J15" s="87"/>
       <c r="K15" s="87"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="71"/>
-      <c r="P15" s="67"/>
+      <c r="L15" s="107"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="100"/>
+      <c r="P15" s="96"/>
       <c r="Q15" s="24" t="str">
         <f>IF($Q$12="1", IF(ISBLANK($K$5),FIXED(_xlfn.XLOOKUP($C18,Data!$T$6:$T$123,Data!$V$6:$V$123,#N/A),$E$9),FIXED($K$5,$E$9)),IF(ISBLANK($K$5),"Error! Density value not specified!",FIXED($K$5,$E$9)))</f>
         <v>Error! Density value not specified!</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="113"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="81"/>
+      <c r="A16" s="122"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="109"/>
       <c r="D16" s="87"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="84"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="112"/>
       <c r="G16" s="87"/>
       <c r="H16" s="87"/>
       <c r="I16" s="87"/>
       <c r="J16" s="87"/>
       <c r="K16" s="87"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="69"/>
-      <c r="O16" s="71"/>
-      <c r="P16" s="67"/>
+      <c r="L16" s="107"/>
+      <c r="M16" s="96"/>
+      <c r="N16" s="98"/>
+      <c r="O16" s="100"/>
+      <c r="P16" s="96"/>
       <c r="Q16" s="24"/>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="114"/>
-      <c r="B17" s="90"/>
-      <c r="C17" s="82"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="110"/>
       <c r="D17" s="88"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="85"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="113"/>
       <c r="G17" s="88"/>
       <c r="H17" s="88"/>
       <c r="I17" s="88"/>
       <c r="J17" s="88"/>
       <c r="K17" s="88"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="68"/>
-      <c r="N17" s="70"/>
-      <c r="O17" s="72"/>
-      <c r="P17" s="68"/>
+      <c r="L17" s="107"/>
+      <c r="M17" s="97"/>
+      <c r="N17" s="99"/>
+      <c r="O17" s="101"/>
+      <c r="P17" s="97"/>
       <c r="Q17" s="24" t="s">
         <v>389</v>
       </c>
@@ -4280,7 +4292,7 @@
         <f>IF(ISBLANK($B18), "",H18/ I18)</f>
         <v/>
       </c>
-      <c r="L18" s="79"/>
+      <c r="L18" s="107"/>
       <c r="M18" s="14" t="str" cm="1">
         <f t="array" ref="M18:N29">_xlfn._xlws.SORT(G18:INDEX(G18:H29,Q12,2),1,1,FALSE)</f>
         <v/>
@@ -4340,7 +4352,7 @@
         <f t="shared" ref="K19:K29" si="5">IF(ISBLANK($B19), "",H19/ I19)</f>
         <v/>
       </c>
-      <c r="L19" s="79"/>
+      <c r="L19" s="107"/>
       <c r="M19" s="14" t="str">
         <v/>
       </c>
@@ -4399,7 +4411,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L20" s="79"/>
+      <c r="L20" s="107"/>
       <c r="M20" s="14" t="str">
         <v/>
       </c>
@@ -4458,7 +4470,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L21" s="79"/>
+      <c r="L21" s="107"/>
       <c r="M21" s="14" t="str">
         <v/>
       </c>
@@ -4517,7 +4529,7 @@
         <f t="shared" ref="K22:K23" si="9">IF(ISBLANK($B22), "",H22/ I22)</f>
         <v/>
       </c>
-      <c r="L22" s="79"/>
+      <c r="L22" s="107"/>
       <c r="M22" s="14" t="str">
         <v/>
       </c>
@@ -4576,7 +4588,7 @@
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="L23" s="79"/>
+      <c r="L23" s="107"/>
       <c r="M23" s="14" t="str">
         <v/>
       </c>
@@ -4635,7 +4647,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L24" s="79"/>
+      <c r="L24" s="107"/>
       <c r="M24" s="14" t="str">
         <v/>
       </c>
@@ -4694,7 +4706,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L25" s="79"/>
+      <c r="L25" s="107"/>
       <c r="M25" s="14" t="str">
         <v/>
       </c>
@@ -4753,7 +4765,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L26" s="79"/>
+      <c r="L26" s="107"/>
       <c r="M26" s="14" t="str">
         <v/>
       </c>
@@ -4812,7 +4824,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L27" s="79"/>
+      <c r="L27" s="107"/>
       <c r="M27" s="14" t="str">
         <v/>
       </c>
@@ -4871,7 +4883,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L28" s="79"/>
+      <c r="L28" s="107"/>
       <c r="M28" s="14" t="str">
         <v/>
       </c>
@@ -4930,7 +4942,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L29" s="80"/>
+      <c r="L29" s="108"/>
       <c r="M29" s="15" t="str">
         <v/>
       </c>
@@ -4951,35 +4963,35 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="91" t="s">
+      <c r="B30" s="66" t="s">
         <v>408</v>
       </c>
-      <c r="E30" s="91" t="s">
+      <c r="E30" s="66" t="s">
         <v>398</v>
       </c>
-      <c r="J30" s="91" t="s">
+      <c r="J30" s="66" t="s">
         <v>393</v>
       </c>
-      <c r="K30" s="91" t="s">
+      <c r="K30" s="66" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="92"/>
-      <c r="E31" s="92"/>
+      <c r="B31" s="67"/>
+      <c r="E31" s="67"/>
       <c r="G31" s="53"/>
-      <c r="J31" s="92"/>
-      <c r="K31" s="92"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
       <c r="P31" s="3"/>
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="92"/>
-      <c r="E32" s="92"/>
+      <c r="B32" s="67"/>
+      <c r="E32" s="67"/>
       <c r="J32" s="41">
         <f>SUM(J18:J29)</f>
         <v>0</v>
       </c>
-      <c r="K32" s="92"/>
+      <c r="K32" s="67"/>
       <c r="P32" s="3"/>
     </row>
     <row r="33" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4991,7 +5003,7 @@
         <f>SUM(E18:E29)</f>
         <v>0</v>
       </c>
-      <c r="K33" s="92"/>
+      <c r="K33" s="67"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
@@ -5021,15 +5033,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="35">
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A3:P3"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="E12:E17"/>
-    <mergeCell ref="D12:D17"/>
-    <mergeCell ref="G7:P7"/>
-    <mergeCell ref="A10:P10"/>
-    <mergeCell ref="A11:P11"/>
-    <mergeCell ref="F9:P9"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="L5:P5"/>
+    <mergeCell ref="D6:P6"/>
+    <mergeCell ref="F8:P8"/>
+    <mergeCell ref="L12:L29"/>
+    <mergeCell ref="P14:P17"/>
+    <mergeCell ref="F12:F17"/>
+    <mergeCell ref="G12:G17"/>
+    <mergeCell ref="I12:I17"/>
+    <mergeCell ref="K12:K17"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A1:P1"/>
@@ -5046,16 +5059,15 @@
     <mergeCell ref="M14:M17"/>
     <mergeCell ref="N14:N17"/>
     <mergeCell ref="O14:O17"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="L5:P5"/>
-    <mergeCell ref="D6:P6"/>
-    <mergeCell ref="F8:P8"/>
-    <mergeCell ref="L12:L29"/>
-    <mergeCell ref="P14:P17"/>
-    <mergeCell ref="F12:F17"/>
-    <mergeCell ref="G12:G17"/>
-    <mergeCell ref="I12:I17"/>
-    <mergeCell ref="K12:K17"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A3:P3"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="E12:E17"/>
+    <mergeCell ref="D12:D17"/>
+    <mergeCell ref="G7:P7"/>
+    <mergeCell ref="A10:P10"/>
+    <mergeCell ref="A11:P11"/>
+    <mergeCell ref="F9:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5079,102 +5091,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="133" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="I1" s="125" t="s">
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="I1" s="131" t="s">
         <v>376</v>
       </c>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="P1" s="124" t="s">
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="P1" s="130" t="s">
         <v>375</v>
       </c>
-      <c r="Q1" s="124"/>
-      <c r="S1" s="125" t="s">
+      <c r="Q1" s="130"/>
+      <c r="S1" s="131" t="s">
         <v>379</v>
       </c>
-      <c r="T1" s="126"/>
-      <c r="U1" s="126"/>
-      <c r="V1" s="126"/>
+      <c r="T1" s="132"/>
+      <c r="U1" s="132"/>
+      <c r="V1" s="132"/>
     </row>
     <row r="2" spans="1:26" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
-      <c r="P2" s="124"/>
-      <c r="Q2" s="124"/>
-      <c r="S2" s="126"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="P2" s="130"/>
+      <c r="Q2" s="130"/>
+      <c r="S2" s="132"/>
+      <c r="T2" s="132"/>
+      <c r="U2" s="132"/>
+      <c r="V2" s="132"/>
     </row>
     <row r="3" spans="1:26" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="128"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="I3" s="125"/>
-      <c r="J3" s="125"/>
-      <c r="K3" s="125"/>
-      <c r="L3" s="125"/>
-      <c r="M3" s="125"/>
-      <c r="N3" s="125"/>
-      <c r="P3" s="124"/>
-      <c r="Q3" s="124"/>
-      <c r="S3" s="126"/>
-      <c r="T3" s="126"/>
-      <c r="U3" s="126"/>
-      <c r="V3" s="126"/>
+      <c r="B3" s="134"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="131"/>
+      <c r="M3" s="131"/>
+      <c r="N3" s="131"/>
+      <c r="P3" s="130"/>
+      <c r="Q3" s="130"/>
+      <c r="S3" s="132"/>
+      <c r="T3" s="132"/>
+      <c r="U3" s="132"/>
+      <c r="V3" s="132"/>
     </row>
     <row r="4" spans="1:26" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="129" t="s">
+      <c r="A4" s="135" t="s">
         <v>250</v>
       </c>
-      <c r="B4" s="129"/>
-      <c r="C4" s="129"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="125"/>
-      <c r="M4" s="125"/>
-      <c r="N4" s="125"/>
-      <c r="P4" s="124"/>
-      <c r="Q4" s="124"/>
-      <c r="S4" s="126"/>
-      <c r="T4" s="126"/>
-      <c r="U4" s="126"/>
-      <c r="V4" s="126"/>
+      <c r="B4" s="135"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="135"/>
+      <c r="F4" s="135"/>
+      <c r="G4" s="135"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="131"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="131"/>
+      <c r="N4" s="131"/>
+      <c r="P4" s="130"/>
+      <c r="Q4" s="130"/>
+      <c r="S4" s="132"/>
+      <c r="T4" s="132"/>
+      <c r="U4" s="132"/>
+      <c r="V4" s="132"/>
     </row>
     <row r="5" spans="1:26" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
Updated CatSim material calculator to v1.1.
</commit_message>
<xml_diff>
--- a/tools/CatSim material calculator.xlsx
+++ b/tools/CatSim material calculator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\200003237\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\200003237\Documents\GitHub\documentation\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D65AE8-C0BA-4026-8EBA-94F622BF552A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E98E7F-E3B5-4FD3-912B-A729234F646C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14610" xr2:uid="{B8F9F76C-33C1-418E-8852-058650A875FE}"/>
   </bookViews>
@@ -1625,9 +1625,9 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="169" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
-    <numFmt numFmtId="177" formatCode="0.00000000000"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="0.00000000000"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -2125,7 +2125,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2250,236 +2250,14 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2491,13 +2269,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2535,7 +2313,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2547,37 +2325,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2606,8 +2363,42 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2617,9 +2408,219 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2984,68 +2985,68 @@
       <c r="L1" s="31"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
+      <c r="A2" s="128"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
     </row>
     <row r="3" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="129" t="s">
         <v>387</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
     </row>
     <row r="4" spans="1:12" s="51" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="133" t="s">
         <v>416</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="126" t="s">
         <v>388</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="127"/>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="126" t="s">
         <v>413</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="127"/>
     </row>
     <row r="7" spans="1:12" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="126" t="s">
         <v>414</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
+      <c r="B7" s="127"/>
+      <c r="C7" s="127"/>
     </row>
     <row r="8" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="131" t="s">
         <v>415</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="131" t="s">
+      <c r="A10" s="123" t="s">
         <v>422</v>
       </c>
-      <c r="B10" s="132"/>
-      <c r="C10" s="133"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="125"/>
     </row>
     <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>423</v>
       </c>
-      <c r="B11" s="130">
+      <c r="B11" s="60">
         <v>44672</v>
       </c>
-      <c r="C11" s="207" t="s">
+      <c r="C11" s="122" t="s">
         <v>470</v>
       </c>
     </row>
@@ -3067,10 +3068,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE334929-57FE-4A9D-B51A-4CE49032E816}">
-  <dimension ref="A1:R64"/>
+  <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3088,108 +3089,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="137" t="s">
         <v>405</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="203" t="s">
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="134" t="s">
         <v>466</v>
       </c>
-      <c r="G1" s="204"/>
-      <c r="H1" s="204"/>
-      <c r="I1" s="204"/>
-      <c r="J1" s="204"/>
-      <c r="K1" s="204"/>
-      <c r="L1" s="204"/>
-      <c r="M1" s="204"/>
-      <c r="N1" s="205"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
+      <c r="N1" s="136"/>
       <c r="O1" s="28" t="s">
         <v>257</v>
       </c>
       <c r="P1" s="45"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="144" t="s">
         <v>382</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="144"/>
+      <c r="N2" s="144"/>
       <c r="O2" s="11" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="144" t="s">
         <v>408</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="63"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="166"/>
       <c r="O3" s="12" t="str">
         <f>CONCATENATE("# Made with ",Instructions!A$1, " ",Instructions!B$1, ".")</f>
         <v># Made with CatSim material calculator, version 1.1.</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="144" t="s">
         <v>409</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="63"/>
+      <c r="B4" s="144"/>
+      <c r="C4" s="144"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="144"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
+      <c r="H4" s="144"/>
+      <c r="I4" s="144"/>
+      <c r="J4" s="144"/>
+      <c r="K4" s="144"/>
+      <c r="L4" s="144"/>
+      <c r="M4" s="144"/>
+      <c r="N4" s="166"/>
       <c r="O4" s="23" t="str">
         <f>IF(O12&lt;&gt;"1", CONCATENATE("# Molecular weights from ", Data!$I$1, "."), "")</f>
         <v># Molecular weights from https://www.nist.gov/pml/atomic-weights-and-isotopic-compositions-relative-atomic-masses.</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="145" t="s">
         <v>410</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="75"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="145"/>
+      <c r="K5" s="146"/>
       <c r="L5" s="52">
         <v>1</v>
       </c>
@@ -3203,69 +3204,69 @@
       </c>
     </row>
     <row r="6" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="145" t="s">
         <v>381</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="206" t="s">
+      <c r="B6" s="145"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="167" t="s">
         <v>418</v>
       </c>
-      <c r="E6" s="180"/>
-      <c r="F6" s="180"/>
-      <c r="G6" s="180"/>
-      <c r="H6" s="180"/>
-      <c r="I6" s="180"/>
-      <c r="J6" s="180"/>
-      <c r="K6" s="180"/>
-      <c r="L6" s="180"/>
-      <c r="M6" s="180"/>
-      <c r="N6" s="181"/>
+      <c r="E6" s="168"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="168"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="168"/>
+      <c r="L6" s="168"/>
+      <c r="M6" s="168"/>
+      <c r="N6" s="169"/>
       <c r="O6" s="23" t="str">
         <f>IF($O$12="1", IF(ISBLANK($F$8), "", #N/A), IF(ISBLANK($F$8), "# Material composition source not specified.", CONCATENATE("# Material composition source: ",$F$8)))</f>
         <v># Material composition source: same as density</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="145" t="s">
         <v>377</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="176" t="s">
+      <c r="B7" s="145"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="145"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="157" t="s">
         <v>417</v>
       </c>
-      <c r="H7" s="177"/>
-      <c r="I7" s="177"/>
-      <c r="J7" s="177"/>
-      <c r="K7" s="177"/>
-      <c r="L7" s="177"/>
-      <c r="M7" s="177"/>
-      <c r="N7" s="178"/>
+      <c r="H7" s="158"/>
+      <c r="I7" s="158"/>
+      <c r="J7" s="158"/>
+      <c r="K7" s="158"/>
+      <c r="L7" s="158"/>
+      <c r="M7" s="158"/>
+      <c r="N7" s="159"/>
       <c r="O7" s="24"/>
     </row>
     <row r="8" spans="1:16" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="145" t="s">
         <v>378</v>
       </c>
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="101" t="s">
+      <c r="B8" s="145"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="145"/>
+      <c r="E8" s="145"/>
+      <c r="F8" s="160" t="s">
         <v>380</v>
       </c>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="102"/>
-      <c r="N8" s="103"/>
+      <c r="G8" s="161"/>
+      <c r="H8" s="161"/>
+      <c r="I8" s="161"/>
+      <c r="J8" s="161"/>
+      <c r="K8" s="161"/>
+      <c r="L8" s="161"/>
+      <c r="M8" s="161"/>
+      <c r="N8" s="162"/>
       <c r="O8" s="23" t="str">
         <f>IF($O$12="1","# Elemental material: ", "# Material name:")</f>
         <v># Material name:</v>
@@ -3280,143 +3281,143 @@
       <c r="D9" s="46">
         <v>6</v>
       </c>
-      <c r="E9" s="74" t="s">
+      <c r="E9" s="176" t="s">
         <v>397</v>
       </c>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="75"/>
+      <c r="F9" s="145"/>
+      <c r="G9" s="145"/>
+      <c r="H9" s="145"/>
+      <c r="I9" s="145"/>
+      <c r="J9" s="145"/>
+      <c r="K9" s="145"/>
+      <c r="L9" s="145"/>
+      <c r="M9" s="145"/>
+      <c r="N9" s="146"/>
       <c r="O9" s="23" t="str">
         <f>IF($O$12="1", IF(ISBLANK($G$7),_xlfn.CONCAT("# ",$A$18, " (", $C$18,")"), _xlfn.CONCAT("# ", $G$7)), IF(ISBLANK($G$7),"# not specified", _xlfn.CONCAT("# ", $G$7)))</f>
         <v># water</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="144" t="s">
         <v>379</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="144"/>
+      <c r="D10" s="144"/>
+      <c r="E10" s="144"/>
+      <c r="F10" s="144"/>
+      <c r="G10" s="144"/>
+      <c r="H10" s="144"/>
+      <c r="I10" s="144"/>
+      <c r="J10" s="144"/>
+      <c r="K10" s="144"/>
+      <c r="L10" s="144"/>
+      <c r="M10" s="144"/>
+      <c r="N10" s="144"/>
       <c r="O10" s="24"/>
     </row>
     <row r="11" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="145" t="s">
         <v>265</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="64"/>
-      <c r="N11" s="64"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="145"/>
+      <c r="E11" s="145"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="145"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="145"/>
+      <c r="K11" s="145"/>
+      <c r="L11" s="145"/>
+      <c r="M11" s="145"/>
+      <c r="N11" s="145"/>
       <c r="O11" s="24" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="147" t="s">
         <v>399</v>
       </c>
-      <c r="B12" s="92"/>
-      <c r="C12" s="84" t="s">
+      <c r="B12" s="148"/>
+      <c r="C12" s="185" t="s">
         <v>256</v>
       </c>
-      <c r="D12" s="104" t="s">
+      <c r="D12" s="163" t="s">
         <v>259</v>
       </c>
-      <c r="E12" s="104" t="s">
+      <c r="E12" s="163" t="s">
         <v>391</v>
       </c>
-      <c r="F12" s="104" t="s">
+      <c r="F12" s="163" t="s">
         <v>392</v>
       </c>
-      <c r="G12" s="76"/>
-      <c r="H12" s="104" t="s">
+      <c r="G12" s="177"/>
+      <c r="H12" s="163" t="s">
         <v>393</v>
       </c>
-      <c r="I12" s="104" t="s">
+      <c r="I12" s="163" t="s">
         <v>389</v>
       </c>
-      <c r="J12" s="79"/>
-      <c r="K12" s="95" t="s">
+      <c r="J12" s="180"/>
+      <c r="K12" s="151" t="s">
         <v>262</v>
       </c>
-      <c r="L12" s="96"/>
-      <c r="M12" s="99" t="s">
+      <c r="L12" s="152"/>
+      <c r="M12" s="155" t="s">
         <v>261</v>
       </c>
-      <c r="N12" s="95"/>
+      <c r="N12" s="151"/>
       <c r="O12" s="23" t="str">
         <f>IF(COUNTA(A18:A29)&lt;&gt;COUNTA(B18:B29),"Error! Different number of entries for Symbol and Number of atoms per molecule.", _xlfn.VALUETOTEXT(COUNTA(B18:B29)))</f>
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="93"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="105"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="97"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="97"/>
+      <c r="A13" s="149"/>
+      <c r="B13" s="150"/>
+      <c r="C13" s="186"/>
+      <c r="D13" s="164"/>
+      <c r="E13" s="164"/>
+      <c r="F13" s="164"/>
+      <c r="G13" s="178"/>
+      <c r="H13" s="164"/>
+      <c r="I13" s="164"/>
+      <c r="J13" s="181"/>
+      <c r="K13" s="153"/>
+      <c r="L13" s="154"/>
+      <c r="M13" s="156"/>
+      <c r="N13" s="153"/>
       <c r="O13" s="24"/>
     </row>
     <row r="14" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="82" t="s">
+      <c r="A14" s="183" t="s">
         <v>263</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="140" t="s">
         <v>406</v>
       </c>
-      <c r="C14" s="85"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="105"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="68" t="s">
+      <c r="C14" s="186"/>
+      <c r="D14" s="164"/>
+      <c r="E14" s="164"/>
+      <c r="F14" s="164"/>
+      <c r="G14" s="178"/>
+      <c r="H14" s="164"/>
+      <c r="I14" s="164"/>
+      <c r="J14" s="181"/>
+      <c r="K14" s="170" t="s">
         <v>259</v>
       </c>
-      <c r="L14" s="70" t="s">
+      <c r="L14" s="172" t="s">
         <v>389</v>
       </c>
-      <c r="M14" s="72" t="s">
+      <c r="M14" s="174" t="s">
         <v>259</v>
       </c>
-      <c r="N14" s="68" t="s">
+      <c r="N14" s="170" t="s">
         <v>389</v>
       </c>
       <c r="O14" s="24" t="str">
@@ -3425,57 +3426,57 @@
       </c>
     </row>
     <row r="15" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="82"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="85"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="80"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="70"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="68"/>
+      <c r="A15" s="183"/>
+      <c r="B15" s="140"/>
+      <c r="C15" s="186"/>
+      <c r="D15" s="164"/>
+      <c r="E15" s="164"/>
+      <c r="F15" s="164"/>
+      <c r="G15" s="178"/>
+      <c r="H15" s="164"/>
+      <c r="I15" s="164"/>
+      <c r="J15" s="181"/>
+      <c r="K15" s="170"/>
+      <c r="L15" s="172"/>
+      <c r="M15" s="174"/>
+      <c r="N15" s="170"/>
       <c r="O15" s="24" t="str">
         <f>IF($O$12="1", IF(ISBLANK($L$5),FIXED(_xlfn.XLOOKUP($A18,Data!$T$6:$T$123,Data!$V$6:$V$123,#N/A),$D$9),FIXED($L$5,$D$9)),IF(ISBLANK($L$5),"Error! Density value not specified!",FIXED($L$5,$D$9)))</f>
         <v>1.000000</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="82"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="70"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="68"/>
+      <c r="A16" s="183"/>
+      <c r="B16" s="140"/>
+      <c r="C16" s="186"/>
+      <c r="D16" s="164"/>
+      <c r="E16" s="164"/>
+      <c r="F16" s="164"/>
+      <c r="G16" s="178"/>
+      <c r="H16" s="164"/>
+      <c r="I16" s="164"/>
+      <c r="J16" s="181"/>
+      <c r="K16" s="170"/>
+      <c r="L16" s="172"/>
+      <c r="M16" s="174"/>
+      <c r="N16" s="170"/>
       <c r="O16" s="24"/>
     </row>
     <row r="17" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="83"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="69"/>
+      <c r="A17" s="184"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="187"/>
+      <c r="D17" s="165"/>
+      <c r="E17" s="165"/>
+      <c r="F17" s="165"/>
+      <c r="G17" s="178"/>
+      <c r="H17" s="165"/>
+      <c r="I17" s="165"/>
+      <c r="J17" s="181"/>
+      <c r="K17" s="171"/>
+      <c r="L17" s="173"/>
+      <c r="M17" s="175"/>
+      <c r="N17" s="171"/>
       <c r="O17" s="24" t="s">
         <v>386</v>
       </c>
@@ -3503,7 +3504,7 @@
         <f>IF(ISBLANK($A18), "", B18*E18)</f>
         <v>2.0159500000000001</v>
       </c>
-      <c r="G18" s="77"/>
+      <c r="G18" s="178"/>
       <c r="H18" s="6">
         <f>D18</f>
         <v>1</v>
@@ -3512,7 +3513,7 @@
         <f>IF(ISBLANK($B18), "", F18/F$33)</f>
         <v>0.11190179485827366</v>
       </c>
-      <c r="J18" s="80"/>
+      <c r="J18" s="181"/>
       <c r="K18" s="14" cm="1">
         <f t="array" ref="K18:L19">_xlfn._xlws.SORT(H18:INDEX(H18:I29,O12,2),1,1,FALSE)</f>
         <v>1</v>
@@ -3556,7 +3557,7 @@
         <f>IF(ISBLANK($A19), "", B19*E19)</f>
         <v>15.9994</v>
       </c>
-      <c r="G19" s="77"/>
+      <c r="G19" s="178"/>
       <c r="H19" s="6">
         <f t="shared" ref="H19:H29" si="0">D19</f>
         <v>8</v>
@@ -3565,7 +3566,7 @@
         <f>IF(ISBLANK($B19), "", F19/F$33)</f>
         <v>0.88809820514172644</v>
       </c>
-      <c r="J19" s="80"/>
+      <c r="J19" s="181"/>
       <c r="K19" s="14">
         <v>8</v>
       </c>
@@ -3587,7 +3588,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
-      <c r="B20" s="154"/>
+      <c r="B20" s="81"/>
       <c r="C20" s="6" t="str">
         <f>IF(ISBLANK($A20), "", _xlfn.XLOOKUP($A20,Data!$B$6:$B$123,Data!$A$6:$A$123,#N/A))</f>
         <v/>
@@ -3604,7 +3605,7 @@
         <f>IF(ISBLANK($A20), "", B20*E20)</f>
         <v/>
       </c>
-      <c r="G20" s="77"/>
+      <c r="G20" s="178"/>
       <c r="H20" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3613,7 +3614,7 @@
         <f>IF(ISBLANK($B20), "", F20/F$33)</f>
         <v/>
       </c>
-      <c r="J20" s="80"/>
+      <c r="J20" s="181"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
       <c r="M20" s="8" t="str">
@@ -3631,7 +3632,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
-      <c r="B21" s="154"/>
+      <c r="B21" s="81"/>
       <c r="C21" s="6" t="str">
         <f>IF(ISBLANK($A21), "", _xlfn.XLOOKUP($A21,Data!$B$6:$B$123,Data!$A$6:$A$123,#N/A))</f>
         <v/>
@@ -3648,7 +3649,7 @@
         <f>IF(ISBLANK($A21), "", B21*E21)</f>
         <v/>
       </c>
-      <c r="G21" s="77"/>
+      <c r="G21" s="178"/>
       <c r="H21" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3657,7 +3658,7 @@
         <f>IF(ISBLANK($B21), "", F21/F$33)</f>
         <v/>
       </c>
-      <c r="J21" s="80"/>
+      <c r="J21" s="181"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
       <c r="M21" s="8" t="str">
@@ -3692,7 +3693,7 @@
         <f t="shared" ref="F22:F29" si="3">IF(ISBLANK($A22), "", B22*E22)</f>
         <v/>
       </c>
-      <c r="G22" s="77"/>
+      <c r="G22" s="178"/>
       <c r="H22" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3701,7 +3702,7 @@
         <f t="shared" ref="I22:I29" si="4">IF(ISBLANK($B22), "", F22/F$33)</f>
         <v/>
       </c>
-      <c r="J22" s="80"/>
+      <c r="J22" s="181"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
       <c r="M22" s="8" t="str">
@@ -3736,7 +3737,7 @@
         <f t="shared" ref="F23:F24" si="5">IF(ISBLANK($A23), "", B23*E23)</f>
         <v/>
       </c>
-      <c r="G23" s="77"/>
+      <c r="G23" s="178"/>
       <c r="H23" s="6" t="str">
         <f t="shared" ref="H23:H24" si="6">D23</f>
         <v/>
@@ -3745,7 +3746,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J23" s="80"/>
+      <c r="J23" s="181"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
       <c r="M23" s="8" t="str">
@@ -3780,7 +3781,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="G24" s="77"/>
+      <c r="G24" s="178"/>
       <c r="H24" s="6" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3789,7 +3790,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J24" s="80"/>
+      <c r="J24" s="181"/>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
       <c r="M24" s="8" t="str">
@@ -3824,7 +3825,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="G25" s="77"/>
+      <c r="G25" s="178"/>
       <c r="H25" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3833,7 +3834,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J25" s="80"/>
+      <c r="J25" s="181"/>
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
       <c r="M25" s="8" t="str">
@@ -3868,7 +3869,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="G26" s="77"/>
+      <c r="G26" s="178"/>
       <c r="H26" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3877,7 +3878,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J26" s="80"/>
+      <c r="J26" s="181"/>
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
       <c r="M26" s="8" t="str">
@@ -3912,7 +3913,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="G27" s="77"/>
+      <c r="G27" s="178"/>
       <c r="H27" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3921,7 +3922,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J27" s="80"/>
+      <c r="J27" s="181"/>
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
       <c r="M27" s="8" t="str">
@@ -3956,7 +3957,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="G28" s="77"/>
+      <c r="G28" s="178"/>
       <c r="H28" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3965,7 +3966,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J28" s="80"/>
+      <c r="J28" s="181"/>
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
       <c r="M28" s="8" t="str">
@@ -4000,7 +4001,7 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="G29" s="78"/>
+      <c r="G29" s="179"/>
       <c r="H29" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4009,7 +4010,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J29" s="81"/>
+      <c r="J29" s="182"/>
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
       <c r="M29" s="9" t="str">
@@ -4026,34 +4027,34 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="89" t="s">
+      <c r="F30" s="142" t="s">
         <v>407</v>
       </c>
-      <c r="M30" s="155" t="s">
+      <c r="M30" s="82" t="s">
         <v>436</v>
       </c>
-      <c r="N30" s="172"/>
-      <c r="O30" s="156"/>
+      <c r="N30" s="99"/>
+      <c r="O30" s="83"/>
       <c r="P30" s="3"/>
     </row>
     <row r="31" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F31" s="90"/>
-      <c r="M31" s="166" t="s">
+      <c r="F31" s="143"/>
+      <c r="M31" s="93" t="s">
         <v>469</v>
       </c>
-      <c r="N31" s="157"/>
-      <c r="O31" s="158"/>
+      <c r="N31" s="84"/>
+      <c r="O31" s="85"/>
       <c r="P31" s="3"/>
     </row>
     <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F32" s="90"/>
-      <c r="M32" s="173">
+      <c r="F32" s="143"/>
+      <c r="M32" s="100">
         <v>20</v>
       </c>
-      <c r="N32" s="157" t="s">
+      <c r="N32" s="84" t="s">
         <v>437</v>
       </c>
-      <c r="O32" s="158"/>
+      <c r="O32" s="85"/>
       <c r="P32" s="53"/>
       <c r="Q32" s="53"/>
       <c r="R32" s="53"/>
@@ -4063,11 +4064,11 @@
         <f>SUM(F18:F29)</f>
         <v>18.015349999999998</v>
       </c>
-      <c r="M33" s="166" t="s">
+      <c r="M33" s="93" t="s">
         <v>444</v>
       </c>
-      <c r="N33" s="157"/>
-      <c r="O33" s="158">
+      <c r="N33" s="84"/>
+      <c r="O33" s="85">
         <f>$N$43</f>
         <v>0.9981899999999998</v>
       </c>
@@ -4077,11 +4078,11 @@
     </row>
     <row r="34" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F34" s="3"/>
-      <c r="M34" s="166" t="s">
+      <c r="M34" s="93" t="s">
         <v>431</v>
       </c>
-      <c r="N34" s="157"/>
-      <c r="O34" s="158" t="s">
+      <c r="N34" s="84"/>
+      <c r="O34" s="85" t="s">
         <v>438</v>
       </c>
       <c r="P34" s="53"/>
@@ -4089,11 +4090,11 @@
       <c r="R34" s="53"/>
     </row>
     <row r="35" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="M35" s="166" t="s">
+      <c r="M35" s="93" t="s">
         <v>426</v>
       </c>
-      <c r="N35" s="157"/>
-      <c r="O35" s="159" t="str">
+      <c r="N35" s="84"/>
+      <c r="O35" s="86" t="str">
         <f xml:space="preserve"> _xlfn.CONCAT("water at ", $M$32, " deg C, with ", ROUND(100*$L$20, 6), "% iodine (", ROUND($N$44, 6), " ", $O$44, ")")</f>
         <v>water at 20 deg C, with 0% iodine (0 mg iodine/mL water-iodine solution)</v>
       </c>
@@ -4101,232 +4102,232 @@
       <c r="Q35" s="53"/>
       <c r="R35" s="53"/>
     </row>
-    <row r="36" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M36" s="166" t="s">
+    <row r="36" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="M36" s="93" t="s">
         <v>432</v>
       </c>
-      <c r="N36" s="157"/>
-      <c r="O36" s="159" t="str">
+      <c r="N36" s="84"/>
+      <c r="O36" s="86" t="str">
         <f>CONCATENATE("modified water_",$M$32,"C")</f>
         <v>modified water_20C</v>
       </c>
+      <c r="P36" s="54"/>
+      <c r="Q36" s="54"/>
+      <c r="R36" s="54"/>
     </row>
     <row r="37" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M37" s="166" t="s">
+      <c r="M37" s="93" t="s">
         <v>461</v>
       </c>
-      <c r="N37" s="157"/>
-      <c r="O37" s="159"/>
-      <c r="P37" s="161"/>
-      <c r="Q37" s="168"/>
-      <c r="R37" s="169" t="s">
+      <c r="N37" s="84"/>
+      <c r="O37" s="86"/>
+    </row>
+    <row r="38" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M38" s="94" t="s">
+        <v>454</v>
+      </c>
+      <c r="N38" s="87"/>
+      <c r="O38" s="88"/>
+      <c r="P38" s="88"/>
+      <c r="Q38" s="95"/>
+      <c r="R38" s="96" t="s">
         <v>447</v>
-      </c>
-    </row>
-    <row r="38" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M38" s="167" t="s">
-        <v>454</v>
-      </c>
-      <c r="N38" s="160"/>
-      <c r="O38" s="161"/>
-      <c r="P38" s="53"/>
-      <c r="Q38" s="163" t="s">
-        <v>446</v>
-      </c>
-      <c r="R38" s="159" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="39" spans="6:18" x14ac:dyDescent="0.25">
       <c r="M39" s="53"/>
-      <c r="N39" s="162">
+      <c r="N39" s="89">
         <f>F33</f>
         <v>18.015349999999998</v>
       </c>
-      <c r="O39" s="159" t="s">
+      <c r="O39" s="86" t="s">
         <v>449</v>
       </c>
       <c r="P39" s="53"/>
-      <c r="Q39" s="170">
-        <v>1</v>
-      </c>
-      <c r="R39" s="183">
-        <v>1.4221740000000001E-4</v>
+      <c r="Q39" s="90" t="s">
+        <v>446</v>
+      </c>
+      <c r="R39" s="86" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="40" spans="6:18" x14ac:dyDescent="0.25">
       <c r="M40" s="53"/>
-      <c r="N40" s="162">
+      <c r="N40" s="89">
         <v>18.015350000000002</v>
       </c>
-      <c r="O40" s="159" t="s">
+      <c r="O40" s="86" t="s">
         <v>445</v>
       </c>
       <c r="P40" s="53"/>
-      <c r="Q40" s="170">
-        <v>2</v>
-      </c>
-      <c r="R40" s="183">
-        <v>2.8443469999999999E-4</v>
+      <c r="Q40" s="97">
+        <v>1</v>
+      </c>
+      <c r="R40" s="102">
+        <v>1.4221740000000001E-4</v>
       </c>
     </row>
     <row r="41" spans="6:18" x14ac:dyDescent="0.25">
       <c r="M41" s="53"/>
-      <c r="N41" s="162">
+      <c r="N41" s="89">
         <f>N39/N40</f>
         <v>0.99999999999999978</v>
       </c>
-      <c r="O41" s="159" t="s">
+      <c r="O41" s="86" t="s">
         <v>453</v>
       </c>
       <c r="P41" s="53"/>
-      <c r="Q41" s="170">
-        <v>5</v>
-      </c>
-      <c r="R41" s="183">
-        <v>7.1108680000000004E-4</v>
+      <c r="Q41" s="97">
+        <v>2</v>
+      </c>
+      <c r="R41" s="102">
+        <v>2.8443469999999999E-4</v>
       </c>
     </row>
     <row r="42" spans="6:18" x14ac:dyDescent="0.25">
       <c r="M42" s="53"/>
-      <c r="N42" s="162">
+      <c r="N42" s="89">
         <f>IF($M$32 = 0, 0.99989, IF($M$32 = 20, 0.99819, IF($M$32 = 37, 0.99336)))</f>
         <v>0.99819000000000002</v>
       </c>
-      <c r="O42" s="159" t="s">
+      <c r="O42" s="86" t="s">
         <v>439</v>
       </c>
       <c r="P42" s="53"/>
-      <c r="Q42" s="170">
-        <v>10</v>
-      </c>
-      <c r="R42" s="183">
-        <v>1.4221735000000001E-3</v>
+      <c r="Q42" s="97">
+        <v>5</v>
+      </c>
+      <c r="R42" s="102">
+        <v>7.1108680000000004E-4</v>
       </c>
     </row>
     <row r="43" spans="6:18" x14ac:dyDescent="0.25">
       <c r="M43" s="53"/>
-      <c r="N43" s="162">
+      <c r="N43" s="89">
         <f>N41*N42</f>
         <v>0.9981899999999998</v>
       </c>
-      <c r="O43" s="159" t="s">
+      <c r="O43" s="86" t="s">
         <v>442</v>
       </c>
       <c r="P43" s="53"/>
-      <c r="Q43" s="170">
-        <v>15</v>
-      </c>
-      <c r="R43" s="183">
-        <v>2.1332602000000002E-3</v>
+      <c r="Q43" s="97">
+        <v>10</v>
+      </c>
+      <c r="R43" s="102">
+        <v>1.4221735000000001E-3</v>
       </c>
     </row>
     <row r="44" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N44" s="182">
+      <c r="N44" s="101">
         <f>1000*(N43-N42)</f>
         <v>-2.2204460492503131E-13</v>
       </c>
-      <c r="O44" s="165" t="s">
+      <c r="O44" s="92" t="s">
         <v>440</v>
       </c>
       <c r="P44" s="53"/>
-      <c r="Q44" s="170">
+      <c r="Q44" s="97">
+        <v>15</v>
+      </c>
+      <c r="R44" s="102">
+        <v>2.1332602000000002E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="M45" s="104" t="s">
+        <v>456</v>
+      </c>
+      <c r="N45" s="105"/>
+      <c r="O45" s="106"/>
+      <c r="P45" s="53"/>
+      <c r="Q45" s="97">
         <v>20</v>
       </c>
-      <c r="R44" s="183">
+      <c r="R45" s="102">
         <v>2.8443469000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="M45" s="185" t="s">
-        <v>456</v>
-      </c>
-      <c r="N45" s="186"/>
-      <c r="O45" s="187"/>
-      <c r="P45" s="53"/>
-      <c r="Q45" s="170">
+    <row r="46" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M46" s="107" t="s">
+        <v>469</v>
+      </c>
+      <c r="N46" s="108"/>
+      <c r="O46" s="109"/>
+      <c r="P46" s="53"/>
+      <c r="Q46" s="97">
         <v>30</v>
       </c>
-      <c r="R45" s="183">
+      <c r="R46" s="102">
         <v>4.2665204000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M46" s="188" t="s">
-        <v>469</v>
-      </c>
-      <c r="N46" s="189"/>
-      <c r="O46" s="190"/>
-      <c r="P46" s="53"/>
-      <c r="Q46" s="170">
+    <row r="47" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M47" s="100">
+        <v>37</v>
+      </c>
+      <c r="N47" s="108" t="s">
+        <v>437</v>
+      </c>
+      <c r="O47" s="109"/>
+      <c r="P47" s="53"/>
+      <c r="Q47" s="97">
         <v>40</v>
       </c>
-      <c r="R46" s="183">
+      <c r="R47" s="102">
         <v>5.6886938000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M47" s="173">
-        <v>37</v>
-      </c>
-      <c r="N47" s="189" t="s">
-        <v>437</v>
-      </c>
-      <c r="O47" s="190"/>
-      <c r="P47" s="53"/>
-      <c r="Q47" s="170">
-        <v>50</v>
-      </c>
-      <c r="R47" s="183">
-        <v>7.1108673000000004E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M48" s="188" t="s">
+    <row r="48" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="M48" s="107" t="s">
         <v>444</v>
       </c>
-      <c r="N48" s="189"/>
-      <c r="O48" s="190">
+      <c r="N48" s="108"/>
+      <c r="O48" s="109">
         <f>$N$58</f>
         <v>0.9933599999999998</v>
       </c>
       <c r="P48" s="53"/>
-      <c r="Q48" s="164">
+      <c r="Q48" s="97">
+        <v>50</v>
+      </c>
+      <c r="R48" s="102">
+        <v>7.1108673000000004E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="13:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M49" s="107" t="s">
+        <v>431</v>
+      </c>
+      <c r="N49" s="108"/>
+      <c r="O49" s="109" t="s">
+        <v>438</v>
+      </c>
+      <c r="P49" s="53"/>
+      <c r="Q49" s="91">
         <v>100</v>
       </c>
-      <c r="R48" s="184">
+      <c r="R49" s="103">
         <v>1.4221734600000001E-2</v>
       </c>
     </row>
-    <row r="49" spans="13:18" x14ac:dyDescent="0.25">
-      <c r="M49" s="188" t="s">
-        <v>431</v>
-      </c>
-      <c r="N49" s="189"/>
-      <c r="O49" s="190" t="s">
-        <v>438</v>
-      </c>
-      <c r="P49" s="53"/>
-    </row>
     <row r="50" spans="13:18" x14ac:dyDescent="0.25">
-      <c r="M50" s="188" t="s">
+      <c r="M50" s="107" t="s">
         <v>426</v>
       </c>
-      <c r="N50" s="189"/>
-      <c r="O50" s="191" t="str">
+      <c r="N50" s="108"/>
+      <c r="O50" s="110" t="str">
         <f xml:space="preserve"> _xlfn.CONCAT("water at ", $M$32, " deg C, with ", ROUND($N$59, 6), $O$59, " (", ROUND(100*(N56-N57), 6), "  mg/mL NaCl)")</f>
         <v>water at 20 deg C, with 0% NaCl in water-NaCl solution (0.664  mg/mL NaCl)</v>
       </c>
       <c r="P50" s="53"/>
-      <c r="Q50" s="53"/>
-      <c r="R50" s="53"/>
     </row>
     <row r="51" spans="13:18" x14ac:dyDescent="0.25">
-      <c r="M51" s="188" t="s">
+      <c r="M51" s="107" t="s">
         <v>432</v>
       </c>
-      <c r="N51" s="189"/>
-      <c r="O51" s="191" t="str">
+      <c r="N51" s="108"/>
+      <c r="O51" s="110" t="str">
         <f>CONCATENATE("modified water_",$M$32,"C")</f>
         <v>modified water_20C</v>
       </c>
@@ -4335,97 +4336,99 @@
       <c r="R51" s="53"/>
     </row>
     <row r="52" spans="13:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M52" s="188" t="s">
+      <c r="M52" s="107" t="s">
         <v>462</v>
       </c>
-      <c r="N52" s="189"/>
-      <c r="O52" s="191"/>
+      <c r="N52" s="108"/>
+      <c r="O52" s="110"/>
       <c r="P52" s="53"/>
+      <c r="Q52" s="53"/>
+      <c r="R52" s="53"/>
     </row>
     <row r="53" spans="13:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M53" s="192" t="s">
+      <c r="M53" s="111" t="s">
         <v>463</v>
       </c>
-      <c r="N53" s="193"/>
-      <c r="O53" s="194"/>
-      <c r="P53" s="194"/>
-      <c r="Q53" s="198"/>
-      <c r="R53" s="199" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="54" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="N53" s="112"/>
+      <c r="O53" s="113"/>
+      <c r="P53" s="53"/>
+    </row>
+    <row r="54" spans="13:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M54" s="53"/>
-      <c r="N54" s="195">
+      <c r="N54" s="114">
         <f>F33</f>
         <v>18.015349999999998</v>
       </c>
-      <c r="O54" s="191" t="s">
+      <c r="O54" s="110" t="s">
         <v>457</v>
       </c>
-      <c r="P54" s="53"/>
-      <c r="Q54" s="200" t="s">
+      <c r="P54" s="113"/>
+      <c r="Q54" s="117"/>
+      <c r="R54" s="118" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="55" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M55" s="53"/>
+      <c r="N55" s="114">
+        <v>18.015350000000002</v>
+      </c>
+      <c r="O55" s="110" t="s">
+        <v>445</v>
+      </c>
+      <c r="P55" s="53"/>
+      <c r="Q55" s="119" t="s">
         <v>464</v>
       </c>
-      <c r="R54" s="191" t="s">
+      <c r="R55" s="110" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="55" spans="13:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M55" s="53"/>
-      <c r="N55" s="195">
-        <v>18.015350000000002</v>
-      </c>
-      <c r="O55" s="191" t="s">
-        <v>445</v>
-      </c>
-      <c r="P55" s="53"/>
-      <c r="Q55" s="201">
-        <v>0.9</v>
-      </c>
-      <c r="R55" s="202">
-        <v>2.7995749999999999E-3</v>
-      </c>
-    </row>
-    <row r="56" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="13:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M56" s="53"/>
-      <c r="N56" s="195">
+      <c r="N56" s="114">
         <f>N54/N55</f>
         <v>0.99999999999999978</v>
       </c>
-      <c r="O56" s="191" t="s">
+      <c r="O56" s="110" t="s">
         <v>458</v>
       </c>
       <c r="P56" s="53"/>
+      <c r="Q56" s="120">
+        <v>0.9</v>
+      </c>
+      <c r="R56" s="121">
+        <v>2.7995749999999999E-3</v>
+      </c>
     </row>
     <row r="57" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M57" s="53"/>
-      <c r="N57" s="195">
+      <c r="N57" s="114">
         <f>IF($M$47 = 0, 0.99989, IF($M$47 = 20, 0.99819, IF($M$47 = 37, 0.99336)))</f>
         <v>0.99336000000000002</v>
       </c>
-      <c r="O57" s="191" t="s">
+      <c r="O57" s="110" t="s">
         <v>439</v>
       </c>
       <c r="P57" s="53"/>
     </row>
     <row r="58" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M58" s="53"/>
-      <c r="N58" s="195">
+      <c r="N58" s="114">
         <f>N56*N57</f>
         <v>0.9933599999999998</v>
       </c>
-      <c r="O58" s="191" t="s">
+      <c r="O58" s="110" t="s">
         <v>459</v>
       </c>
       <c r="P58" s="53"/>
     </row>
     <row r="59" spans="13:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N59" s="196">
+      <c r="N59" s="115">
         <f>100*(L20+L21)</f>
         <v>0</v>
       </c>
-      <c r="O59" s="197" t="s">
+      <c r="O59" s="116" t="s">
         <v>460</v>
       </c>
       <c r="P59" s="53"/>
@@ -4450,9 +4453,29 @@
       <c r="O64" s="53"/>
       <c r="P64" s="53"/>
     </row>
+    <row r="65" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P65" s="53"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="33">
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="I12:I17"/>
+    <mergeCell ref="H12:H17"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:N6"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="M14:M17"/>
+    <mergeCell ref="N14:N17"/>
+    <mergeCell ref="A11:N11"/>
+    <mergeCell ref="E9:N9"/>
+    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="G12:G29"/>
+    <mergeCell ref="J12:J29"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A10:N10"/>
     <mergeCell ref="F1:N1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B14:B17"/>
@@ -4469,23 +4492,6 @@
     <mergeCell ref="D12:D17"/>
     <mergeCell ref="E12:E17"/>
     <mergeCell ref="F12:F17"/>
-    <mergeCell ref="I12:I17"/>
-    <mergeCell ref="H12:H17"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:N6"/>
-    <mergeCell ref="K14:K17"/>
-    <mergeCell ref="L14:L17"/>
-    <mergeCell ref="M14:M17"/>
-    <mergeCell ref="N14:N17"/>
-    <mergeCell ref="A11:N11"/>
-    <mergeCell ref="E9:N9"/>
-    <mergeCell ref="A4:N4"/>
-    <mergeCell ref="G12:G29"/>
-    <mergeCell ref="J12:J29"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A10:N10"/>
-    <mergeCell ref="C12:C17"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M32 M47" xr:uid="{36745EB9-6DFC-4A18-A2B7-FAB74AA8976B}">
@@ -4526,124 +4532,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="137" t="s">
         <v>405</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="203" t="s">
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="134" t="s">
         <v>467</v>
       </c>
-      <c r="K1" s="204"/>
-      <c r="L1" s="204"/>
-      <c r="M1" s="204"/>
-      <c r="N1" s="204"/>
-      <c r="O1" s="204"/>
-      <c r="P1" s="205"/>
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
+      <c r="N1" s="135"/>
+      <c r="O1" s="135"/>
+      <c r="P1" s="136"/>
       <c r="Q1" s="28" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="188" t="s">
         <v>400</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="166"/>
+      <c r="H2" s="166"/>
+      <c r="I2" s="166"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="166"/>
+      <c r="M2" s="166"/>
+      <c r="N2" s="166"/>
+      <c r="O2" s="166"/>
+      <c r="P2" s="166"/>
       <c r="Q2" s="11" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="188" t="s">
         <v>408</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
+      <c r="L3" s="166"/>
+      <c r="M3" s="166"/>
+      <c r="N3" s="166"/>
+      <c r="O3" s="166"/>
+      <c r="P3" s="166"/>
       <c r="Q3" s="12" t="str">
         <f>CONCATENATE("# Made with ",Instructions!A$1, " ",Instructions!B$1, ".")</f>
         <v># Made with CatSim material calculator, version 1.1.</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="145" t="s">
         <v>409</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="145"/>
+      <c r="J4" s="145"/>
+      <c r="K4" s="145"/>
+      <c r="L4" s="145"/>
+      <c r="M4" s="145"/>
+      <c r="N4" s="145"/>
+      <c r="O4" s="145"/>
+      <c r="P4" s="145"/>
       <c r="Q4" s="23" t="str">
         <f>IF(Q12&lt;&gt;"1", CONCATENATE("# Molecular weights from ", Data!$I$1, "."), "")</f>
         <v># Molecular weights from https://www.nist.gov/pml/atomic-weights-and-isotopic-compositions-relative-atomic-masses.</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="176" t="s">
         <v>411</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="75"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="146"/>
       <c r="K5" s="52">
         <v>1</v>
       </c>
-      <c r="L5" s="174" t="s">
+      <c r="L5" s="200" t="s">
         <v>264</v>
       </c>
-      <c r="M5" s="175"/>
-      <c r="N5" s="175"/>
-      <c r="O5" s="175"/>
-      <c r="P5" s="175"/>
+      <c r="M5" s="201"/>
+      <c r="N5" s="201"/>
+      <c r="O5" s="201"/>
+      <c r="P5" s="201"/>
       <c r="Q5" s="23" t="str">
         <f>IF(AND($Q$12="1",ISBLANK($K$5),ISBLANK($D$6)),CONCATENATE("# Density from ", Data!$S$1, "."), IF(ISBLANK($D$6),"# Density source not specified.",_xlfn.CONCAT("# Density source: ",$D$6)))</f>
         <v># Density source: https://physics.nist.gov/PhysRefData/XrayMassCoef/tab2.html</v>
@@ -4655,21 +4661,21 @@
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="179" t="s">
+      <c r="D6" s="202" t="s">
         <v>418</v>
       </c>
-      <c r="E6" s="180"/>
-      <c r="F6" s="180"/>
-      <c r="G6" s="180"/>
-      <c r="H6" s="180"/>
-      <c r="I6" s="180"/>
-      <c r="J6" s="180"/>
-      <c r="K6" s="180"/>
-      <c r="L6" s="180"/>
-      <c r="M6" s="180"/>
-      <c r="N6" s="180"/>
-      <c r="O6" s="180"/>
-      <c r="P6" s="181"/>
+      <c r="E6" s="168"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="168"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="168"/>
+      <c r="L6" s="168"/>
+      <c r="M6" s="168"/>
+      <c r="N6" s="168"/>
+      <c r="O6" s="168"/>
+      <c r="P6" s="169"/>
       <c r="Q6" s="23" t="str">
         <f>IF(ISBLANK($F$8),IF($Q$12=1,"","# Material composition source not specified."),CONCATENATE("# Material composition source: ",$F$8))</f>
         <v># Material composition source: L18-L19 on "Enter a formula" sheet</v>
@@ -4684,18 +4690,18 @@
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="176" t="s">
+      <c r="G7" s="157" t="s">
         <v>417</v>
       </c>
-      <c r="H7" s="177"/>
-      <c r="I7" s="177"/>
-      <c r="J7" s="177"/>
-      <c r="K7" s="177"/>
-      <c r="L7" s="177"/>
-      <c r="M7" s="177"/>
-      <c r="N7" s="177"/>
-      <c r="O7" s="177"/>
-      <c r="P7" s="177"/>
+      <c r="H7" s="158"/>
+      <c r="I7" s="158"/>
+      <c r="J7" s="158"/>
+      <c r="K7" s="158"/>
+      <c r="L7" s="158"/>
+      <c r="M7" s="158"/>
+      <c r="N7" s="158"/>
+      <c r="O7" s="158"/>
+      <c r="P7" s="158"/>
       <c r="Q7" s="24"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4706,19 +4712,19 @@
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="101" t="s">
+      <c r="F8" s="160" t="s">
         <v>468</v>
       </c>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="102"/>
-      <c r="N8" s="102"/>
-      <c r="O8" s="102"/>
-      <c r="P8" s="102"/>
+      <c r="G8" s="161"/>
+      <c r="H8" s="161"/>
+      <c r="I8" s="161"/>
+      <c r="J8" s="161"/>
+      <c r="K8" s="161"/>
+      <c r="L8" s="161"/>
+      <c r="M8" s="161"/>
+      <c r="N8" s="161"/>
+      <c r="O8" s="161"/>
+      <c r="P8" s="161"/>
       <c r="Q8" s="23" t="str">
         <f>IF($Q$12="1","# Elemental material: ", "# Material name:")</f>
         <v># Material name:</v>
@@ -4734,160 +4740,160 @@
       <c r="E9" s="46">
         <v>6</v>
       </c>
-      <c r="F9" s="117" t="s">
+      <c r="F9" s="191" t="s">
         <v>397</v>
       </c>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="118"/>
-      <c r="J9" s="118"/>
-      <c r="K9" s="118"/>
-      <c r="L9" s="118"/>
-      <c r="M9" s="118"/>
-      <c r="N9" s="118"/>
-      <c r="O9" s="118"/>
-      <c r="P9" s="118"/>
+      <c r="G9" s="192"/>
+      <c r="H9" s="192"/>
+      <c r="I9" s="192"/>
+      <c r="J9" s="192"/>
+      <c r="K9" s="192"/>
+      <c r="L9" s="192"/>
+      <c r="M9" s="192"/>
+      <c r="N9" s="192"/>
+      <c r="O9" s="192"/>
+      <c r="P9" s="192"/>
       <c r="Q9" s="23" t="str">
         <f>IF($Q$12="1", IF(ISBLANK($G$7),_xlfn.CONCAT("# ",$F$18, " (", $C$18,")"), _xlfn.CONCAT("# ", $G$7)), IF(ISBLANK($G$7),"# not specified", _xlfn.CONCAT("# ", $G$7)))</f>
         <v># water</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="115" t="s">
+      <c r="A10" s="188" t="s">
         <v>379</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="63"/>
-      <c r="P10" s="63"/>
+      <c r="B10" s="166"/>
+      <c r="C10" s="166"/>
+      <c r="D10" s="166"/>
+      <c r="E10" s="166"/>
+      <c r="F10" s="166"/>
+      <c r="G10" s="166"/>
+      <c r="H10" s="166"/>
+      <c r="I10" s="166"/>
+      <c r="J10" s="166"/>
+      <c r="K10" s="166"/>
+      <c r="L10" s="166"/>
+      <c r="M10" s="166"/>
+      <c r="N10" s="166"/>
+      <c r="O10" s="166"/>
+      <c r="P10" s="166"/>
       <c r="Q10" s="24"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="176" t="s">
         <v>265</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="64"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="64"/>
-      <c r="P11" s="64"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="145"/>
+      <c r="E11" s="145"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="145"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="145"/>
+      <c r="K11" s="145"/>
+      <c r="L11" s="145"/>
+      <c r="M11" s="145"/>
+      <c r="N11" s="145"/>
+      <c r="O11" s="145"/>
+      <c r="P11" s="145"/>
       <c r="Q11" s="24" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="147" t="s">
         <v>399</v>
       </c>
-      <c r="B12" s="92"/>
-      <c r="C12" s="116" t="s">
+      <c r="B12" s="148"/>
+      <c r="C12" s="189" t="s">
         <v>263</v>
       </c>
-      <c r="D12" s="104" t="s">
+      <c r="D12" s="163" t="s">
         <v>395</v>
       </c>
-      <c r="E12" s="110" t="s">
+      <c r="E12" s="190" t="s">
         <v>396</v>
       </c>
-      <c r="F12" s="84" t="s">
+      <c r="F12" s="185" t="s">
         <v>256</v>
       </c>
-      <c r="G12" s="104" t="s">
+      <c r="G12" s="163" t="s">
         <v>259</v>
       </c>
-      <c r="H12" s="104" t="s">
+      <c r="H12" s="163" t="s">
         <v>402</v>
       </c>
-      <c r="I12" s="104" t="s">
+      <c r="I12" s="163" t="s">
         <v>258</v>
       </c>
-      <c r="J12" s="104" t="s">
+      <c r="J12" s="163" t="s">
         <v>427</v>
       </c>
-      <c r="K12" s="104" t="s">
+      <c r="K12" s="163" t="s">
         <v>390</v>
       </c>
-      <c r="L12" s="79"/>
-      <c r="M12" s="111" t="s">
+      <c r="L12" s="180"/>
+      <c r="M12" s="196" t="s">
         <v>404</v>
       </c>
-      <c r="N12" s="112"/>
-      <c r="O12" s="99" t="s">
+      <c r="N12" s="197"/>
+      <c r="O12" s="155" t="s">
         <v>261</v>
       </c>
-      <c r="P12" s="95"/>
+      <c r="P12" s="151"/>
       <c r="Q12" s="23" t="str">
         <f>IF(COUNTA(A18:A29)&lt;&gt;COUNTA(B18:B29),"Error! Different number of entries for Atomic number and Mass fraction.", _xlfn.VALUETOTEXT(COUNTA(B18:B29)))</f>
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="93"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="105"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="113"/>
-      <c r="N13" s="114"/>
-      <c r="O13" s="100"/>
-      <c r="P13" s="97"/>
+      <c r="A13" s="149"/>
+      <c r="B13" s="150"/>
+      <c r="C13" s="183"/>
+      <c r="D13" s="164"/>
+      <c r="E13" s="140"/>
+      <c r="F13" s="186"/>
+      <c r="G13" s="164"/>
+      <c r="H13" s="164"/>
+      <c r="I13" s="164"/>
+      <c r="J13" s="164"/>
+      <c r="K13" s="164"/>
+      <c r="L13" s="181"/>
+      <c r="M13" s="198"/>
+      <c r="N13" s="199"/>
+      <c r="O13" s="156"/>
+      <c r="P13" s="153"/>
       <c r="Q13" s="24"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="107" t="s">
+      <c r="A14" s="193" t="s">
         <v>259</v>
       </c>
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="190" t="s">
         <v>389</v>
       </c>
-      <c r="C14" s="82"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="105"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="80"/>
-      <c r="M14" s="68" t="s">
+      <c r="C14" s="183"/>
+      <c r="D14" s="164"/>
+      <c r="E14" s="140"/>
+      <c r="F14" s="186"/>
+      <c r="G14" s="164"/>
+      <c r="H14" s="164"/>
+      <c r="I14" s="164"/>
+      <c r="J14" s="164"/>
+      <c r="K14" s="164"/>
+      <c r="L14" s="181"/>
+      <c r="M14" s="170" t="s">
         <v>259</v>
       </c>
-      <c r="N14" s="70" t="s">
+      <c r="N14" s="172" t="s">
         <v>389</v>
       </c>
-      <c r="O14" s="72" t="s">
+      <c r="O14" s="174" t="s">
         <v>259</v>
       </c>
-      <c r="P14" s="68" t="s">
+      <c r="P14" s="170" t="s">
         <v>389</v>
       </c>
       <c r="Q14" s="24" t="str">
@@ -4896,63 +4902,63 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="108"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="80"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="70"/>
-      <c r="O15" s="72"/>
-      <c r="P15" s="68"/>
+      <c r="A15" s="194"/>
+      <c r="B15" s="140"/>
+      <c r="C15" s="183"/>
+      <c r="D15" s="164"/>
+      <c r="E15" s="140"/>
+      <c r="F15" s="186"/>
+      <c r="G15" s="164"/>
+      <c r="H15" s="164"/>
+      <c r="I15" s="164"/>
+      <c r="J15" s="164"/>
+      <c r="K15" s="164"/>
+      <c r="L15" s="181"/>
+      <c r="M15" s="170"/>
+      <c r="N15" s="172"/>
+      <c r="O15" s="174"/>
+      <c r="P15" s="170"/>
       <c r="Q15" s="24" t="str">
         <f>IF($Q$12="1", IF(ISBLANK($K$5),FIXED(_xlfn.XLOOKUP($C18,Data!$T$6:$T$123,Data!$V$6:$V$123,#N/A),$E$9),FIXED($K$5,$E$9)),IF(ISBLANK($K$5),"Error! Density value not specified!",FIXED($K$5,$E$9)))</f>
         <v>1.000000</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="108"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="105"/>
-      <c r="L16" s="80"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="70"/>
-      <c r="O16" s="72"/>
-      <c r="P16" s="68"/>
+      <c r="A16" s="194"/>
+      <c r="B16" s="140"/>
+      <c r="C16" s="183"/>
+      <c r="D16" s="164"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="186"/>
+      <c r="G16" s="164"/>
+      <c r="H16" s="164"/>
+      <c r="I16" s="164"/>
+      <c r="J16" s="164"/>
+      <c r="K16" s="164"/>
+      <c r="L16" s="181"/>
+      <c r="M16" s="170"/>
+      <c r="N16" s="172"/>
+      <c r="O16" s="174"/>
+      <c r="P16" s="170"/>
       <c r="Q16" s="24"/>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="109"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="80"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="71"/>
-      <c r="O17" s="73"/>
-      <c r="P17" s="69"/>
+      <c r="A17" s="195"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="184"/>
+      <c r="D17" s="165"/>
+      <c r="E17" s="141"/>
+      <c r="F17" s="187"/>
+      <c r="G17" s="165"/>
+      <c r="H17" s="165"/>
+      <c r="I17" s="165"/>
+      <c r="J17" s="165"/>
+      <c r="K17" s="165"/>
+      <c r="L17" s="181"/>
+      <c r="M17" s="171"/>
+      <c r="N17" s="173"/>
+      <c r="O17" s="175"/>
+      <c r="P17" s="171"/>
       <c r="Q17" s="24" t="s">
         <v>386</v>
       </c>
@@ -4961,7 +4967,7 @@
       <c r="A18" s="47">
         <v>1</v>
       </c>
-      <c r="B18" s="147">
+      <c r="B18" s="74">
         <v>0.11190179485827366</v>
       </c>
       <c r="C18" s="34" t="str">
@@ -4969,11 +4975,11 @@
         <v>H</v>
       </c>
       <c r="D18" s="43">
-        <f>IF(E18= "","",E18/$E$33)</f>
+        <f t="shared" ref="D18:D29" si="0">IF(E18= "","",E18/$E$33)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="E18" s="141">
-        <f>IF(C18="", "", K18/$K$34)</f>
+      <c r="E18" s="68">
+        <f t="shared" ref="E18:E29" si="1">IF(C18="", "", K18/$K$34)</f>
         <v>2</v>
       </c>
       <c r="F18" s="6" t="str">
@@ -4981,18 +4987,18 @@
         <v>hydrogen</v>
       </c>
       <c r="G18" s="6">
-        <f t="shared" ref="G18:G29" si="0">IF(ISBLANK(A18), "", A18)</f>
+        <f t="shared" ref="G18:G29" si="2">IF(ISBLANK(A18), "", A18)</f>
         <v>1</v>
       </c>
       <c r="H18" s="6">
-        <f>IF($C18="", "", B18/$B$33)</f>
+        <f t="shared" ref="H18:H29" si="3">IF($C18="", "", B18/$B$33)</f>
         <v>0.11190179485827366</v>
       </c>
-      <c r="I18" s="140">
+      <c r="I18" s="67">
         <f>IF($C18="", "", _xlfn.XLOOKUP($C18,Data!$B$6:$B$123,Data!$G$6:$G$123,#N/A))</f>
         <v>1.0079750000000001</v>
       </c>
-      <c r="J18" s="139">
+      <c r="J18" s="66">
         <f>IF(ISBLANK($B18), "",E18*I18)</f>
         <v>2.0159500000000001</v>
       </c>
@@ -5000,7 +5006,7 @@
         <f>IF(ISBLANK($B18), "",H18/ I18)</f>
         <v>0.11101643875916928</v>
       </c>
-      <c r="L18" s="80"/>
+      <c r="L18" s="181"/>
       <c r="M18" s="14" cm="1">
         <f t="array" ref="M18:N19">_xlfn._xlws.SORT(G18:INDEX(G18:H29,Q12,2),1,1,FALSE)</f>
         <v>1</v>
@@ -5025,7 +5031,7 @@
       <c r="A19" s="47">
         <v>8</v>
       </c>
-      <c r="B19" s="147">
+      <c r="B19" s="74">
         <v>0.88809820514172644</v>
       </c>
       <c r="C19" s="34" t="str">
@@ -5033,11 +5039,11 @@
         <v>O</v>
       </c>
       <c r="D19" s="43">
-        <f>IF(E19= "","",E19/$E$33)</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E19" s="141">
-        <f>IF(C19="", "", K19/$K$34)</f>
+      <c r="E19" s="68">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F19" s="6" t="str">
@@ -5045,26 +5051,26 @@
         <v>oxygen</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="H19" s="6">
-        <f>IF($C19="", "", B19/$B$33)</f>
+        <f t="shared" si="3"/>
         <v>0.88809820514172644</v>
       </c>
-      <c r="I19" s="140">
+      <c r="I19" s="67">
         <f>IF($C19="", "", _xlfn.XLOOKUP($C19,Data!$B$6:$B$123,Data!$G$6:$G$123,#N/A))</f>
         <v>15.9994</v>
       </c>
-      <c r="J19" s="139">
-        <f t="shared" ref="J19:J28" si="1">IF(ISBLANK($B19), "",E19*I19)</f>
+      <c r="J19" s="66">
+        <f t="shared" ref="J19:J28" si="4">IF(ISBLANK($B19), "",E19*I19)</f>
         <v>15.9994</v>
       </c>
       <c r="K19" s="37">
-        <f t="shared" ref="K19:K29" si="2">IF(ISBLANK($B19), "",H19/ I19)</f>
+        <f t="shared" ref="K19:K29" si="5">IF(ISBLANK($B19), "",H19/ I19)</f>
         <v>5.5508219379584639E-2</v>
       </c>
-      <c r="L19" s="80"/>
+      <c r="L19" s="181"/>
       <c r="M19" s="14">
         <v>8</v>
       </c>
@@ -5072,11 +5078,11 @@
         <v>0.88809820514172644</v>
       </c>
       <c r="O19" s="8" t="str">
-        <f t="shared" ref="O19:O29" si="3">_xlfn.VALUETOTEXT(M19)</f>
+        <f t="shared" ref="O19:O29" si="6">_xlfn.VALUETOTEXT(M19)</f>
         <v>8</v>
       </c>
       <c r="P19" s="14" t="str">
-        <f t="shared" ref="P19:P29" si="4">IF(O19="", "", FIXED(N19,$E$9))</f>
+        <f t="shared" ref="P19:P29" si="7">IF(O19="", "", FIXED(N19,$E$9))</f>
         <v>0.888098</v>
       </c>
       <c r="Q19" s="24" t="str">
@@ -5086,17 +5092,17 @@
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
-      <c r="B20" s="147"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="34" t="str">
         <f>IF($G20="", "", _xlfn.XLOOKUP($G20,Data!$C$6:$C$123,Data!$B$6:$B$123,#N/A))</f>
         <v/>
       </c>
       <c r="D20" s="43" t="str">
-        <f>IF(E20= "","",E20/$E$33)</f>
-        <v/>
-      </c>
-      <c r="E20" s="141" t="str">
-        <f>IF(C20="", "", K20/$K$34)</f>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E20" s="68" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F20" s="6" t="str">
@@ -5104,34 +5110,34 @@
         <v/>
       </c>
       <c r="G20" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H20" s="6" t="str">
-        <f>IF($C20="", "", B20/$B$33)</f>
-        <v/>
-      </c>
-      <c r="I20" s="140" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I20" s="67" t="str">
         <f>IF($C20="", "", _xlfn.XLOOKUP($C20,Data!$B$6:$B$123,Data!$G$6:$G$123,#N/A))</f>
         <v/>
       </c>
-      <c r="J20" s="139" t="str">
-        <f t="shared" si="1"/>
+      <c r="J20" s="66" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K20" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L20" s="80"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L20" s="181"/>
       <c r="M20" s="14"/>
       <c r="N20" s="14"/>
       <c r="O20" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P20" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q20" s="24" t="str">
@@ -5141,17 +5147,17 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
-      <c r="B21" s="147"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="34" t="str">
         <f>IF($G21="", "", _xlfn.XLOOKUP($G21,Data!$C$6:$C$123,Data!$B$6:$B$123,#N/A))</f>
         <v/>
       </c>
       <c r="D21" s="43" t="str">
-        <f>IF(E21= "","",E21/$E$33)</f>
-        <v/>
-      </c>
-      <c r="E21" s="141" t="str">
-        <f>IF(C21="", "", K21/$K$34)</f>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E21" s="68" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F21" s="6" t="str">
@@ -5159,34 +5165,34 @@
         <v/>
       </c>
       <c r="G21" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H21" s="6" t="str">
-        <f>IF($C21="", "", B21/$B$33)</f>
-        <v/>
-      </c>
-      <c r="I21" s="140" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I21" s="67" t="str">
         <f>IF($C21="", "", _xlfn.XLOOKUP($C21,Data!$B$6:$B$123,Data!$G$6:$G$123,#N/A))</f>
         <v/>
       </c>
-      <c r="J21" s="139" t="str">
-        <f t="shared" si="1"/>
+      <c r="J21" s="66" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K21" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L21" s="80"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L21" s="181"/>
       <c r="M21" s="14"/>
       <c r="N21" s="14"/>
       <c r="O21" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P21" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q21" s="24" t="str">
@@ -5196,17 +5202,17 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
-      <c r="B22" s="147"/>
+      <c r="B22" s="74"/>
       <c r="C22" s="34" t="str">
         <f>IF($G22="", "", _xlfn.XLOOKUP($G22,Data!$C$6:$C$123,Data!$B$6:$B$123,#N/A))</f>
         <v/>
       </c>
       <c r="D22" s="41" t="str">
-        <f>IF(E22= "","",E22/$E$33)</f>
-        <v/>
-      </c>
-      <c r="E22" s="141" t="str">
-        <f>IF(C22="", "", K22/$K$34)</f>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E22" s="68" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F22" s="6" t="str">
@@ -5214,34 +5220,34 @@
         <v/>
       </c>
       <c r="G22" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H22" s="6" t="str">
-        <f>IF($C22="", "", B22/$B$33)</f>
-        <v/>
-      </c>
-      <c r="I22" s="140" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I22" s="67" t="str">
         <f>IF($C22="", "", _xlfn.XLOOKUP($C22,Data!$B$6:$B$123,Data!$G$6:$G$123,#N/A))</f>
         <v/>
       </c>
-      <c r="J22" s="139" t="str">
-        <f t="shared" si="1"/>
+      <c r="J22" s="66" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K22" s="37" t="str">
-        <f t="shared" ref="K22:K23" si="5">IF(ISBLANK($B22), "",H22/ I22)</f>
-        <v/>
-      </c>
-      <c r="L22" s="80"/>
+        <f t="shared" ref="K22:K23" si="8">IF(ISBLANK($B22), "",H22/ I22)</f>
+        <v/>
+      </c>
+      <c r="L22" s="181"/>
       <c r="M22" s="14"/>
       <c r="N22" s="14"/>
       <c r="O22" s="8" t="str">
-        <f t="shared" ref="O22:O23" si="6">_xlfn.VALUETOTEXT(M22)</f>
+        <f t="shared" ref="O22:O23" si="9">_xlfn.VALUETOTEXT(M22)</f>
         <v/>
       </c>
       <c r="P22" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q22" s="24" t="str">
@@ -5251,17 +5257,17 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
-      <c r="B23" s="147"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="34" t="str">
         <f>IF($G23="", "", _xlfn.XLOOKUP($G23,Data!$C$6:$C$123,Data!$B$6:$B$123,#N/A))</f>
         <v/>
       </c>
       <c r="D23" s="41" t="str">
-        <f>IF(E23= "","",E23/$E$33)</f>
-        <v/>
-      </c>
-      <c r="E23" s="141" t="str">
-        <f>IF(C23="", "", K23/$K$34)</f>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E23" s="68" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F23" s="6" t="str">
@@ -5269,34 +5275,34 @@
         <v/>
       </c>
       <c r="G23" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H23" s="6" t="str">
-        <f>IF($C23="", "", B23/$B$33)</f>
-        <v/>
-      </c>
-      <c r="I23" s="140" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I23" s="67" t="str">
         <f>IF($C23="", "", _xlfn.XLOOKUP($C23,Data!$B$6:$B$123,Data!$G$6:$G$123,#N/A))</f>
         <v/>
       </c>
-      <c r="J23" s="139" t="str">
-        <f t="shared" si="1"/>
+      <c r="J23" s="66" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K23" s="37" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="L23" s="80"/>
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="L23" s="181"/>
       <c r="M23" s="14"/>
       <c r="N23" s="14"/>
       <c r="O23" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="P23" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q23" s="24" t="str">
@@ -5306,17 +5312,17 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="47"/>
-      <c r="B24" s="147"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="34" t="str">
         <f>IF($G24="", "", _xlfn.XLOOKUP($G24,Data!$C$6:$C$123,Data!$B$6:$B$123,#N/A))</f>
         <v/>
       </c>
       <c r="D24" s="41" t="str">
-        <f>IF(E24= "","",E24/$E$33)</f>
-        <v/>
-      </c>
-      <c r="E24" s="141" t="str">
-        <f>IF(C24="", "", K24/$K$34)</f>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E24" s="68" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F24" s="6" t="str">
@@ -5324,34 +5330,34 @@
         <v/>
       </c>
       <c r="G24" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H24" s="6" t="str">
-        <f>IF($C24="", "", B24/$B$33)</f>
-        <v/>
-      </c>
-      <c r="I24" s="140" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I24" s="67" t="str">
         <f>IF($C24="", "", _xlfn.XLOOKUP($C24,Data!$B$6:$B$123,Data!$G$6:$G$123,#N/A))</f>
         <v/>
       </c>
-      <c r="J24" s="139" t="str">
-        <f t="shared" si="1"/>
+      <c r="J24" s="66" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K24" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L24" s="80"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L24" s="181"/>
       <c r="M24" s="14"/>
       <c r="N24" s="14"/>
       <c r="O24" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P24" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q24" s="24" t="str">
@@ -5361,17 +5367,17 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
-      <c r="B25" s="147"/>
+      <c r="B25" s="74"/>
       <c r="C25" s="34" t="str">
         <f>IF($G25="", "", _xlfn.XLOOKUP($G25,Data!$C$6:$C$123,Data!$B$6:$B$123,#N/A))</f>
         <v/>
       </c>
       <c r="D25" s="41" t="str">
-        <f>IF(E25= "","",E25/$E$33)</f>
-        <v/>
-      </c>
-      <c r="E25" s="141" t="str">
-        <f>IF(C25="", "", K25/$K$34)</f>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E25" s="68" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F25" s="6" t="str">
@@ -5379,34 +5385,34 @@
         <v/>
       </c>
       <c r="G25" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H25" s="6" t="str">
-        <f>IF($C25="", "", B25/$B$33)</f>
-        <v/>
-      </c>
-      <c r="I25" s="140" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I25" s="67" t="str">
         <f>IF($C25="", "", _xlfn.XLOOKUP($C25,Data!$B$6:$B$123,Data!$G$6:$G$123,#N/A))</f>
         <v/>
       </c>
-      <c r="J25" s="139" t="str">
-        <f t="shared" si="1"/>
+      <c r="J25" s="66" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K25" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L25" s="80"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L25" s="181"/>
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
       <c r="O25" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P25" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q25" s="24" t="str">
@@ -5416,17 +5422,17 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="47"/>
-      <c r="B26" s="147"/>
+      <c r="B26" s="74"/>
       <c r="C26" s="34" t="str">
         <f>IF($G26="", "", _xlfn.XLOOKUP($G26,Data!$C$6:$C$123,Data!$B$6:$B$123,#N/A))</f>
         <v/>
       </c>
       <c r="D26" s="41" t="str">
-        <f>IF(E26= "","",E26/$E$33)</f>
-        <v/>
-      </c>
-      <c r="E26" s="141" t="str">
-        <f>IF(C26="", "", K26/$K$34)</f>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E26" s="68" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F26" s="6" t="str">
@@ -5434,34 +5440,34 @@
         <v/>
       </c>
       <c r="G26" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H26" s="6" t="str">
-        <f>IF($C26="", "", B26/$B$33)</f>
-        <v/>
-      </c>
-      <c r="I26" s="140" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I26" s="67" t="str">
         <f>IF($C26="", "", _xlfn.XLOOKUP($C26,Data!$B$6:$B$123,Data!$G$6:$G$123,#N/A))</f>
         <v/>
       </c>
-      <c r="J26" s="139" t="str">
-        <f t="shared" si="1"/>
+      <c r="J26" s="66" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K26" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L26" s="80"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L26" s="181"/>
       <c r="M26" s="14"/>
       <c r="N26" s="14"/>
       <c r="O26" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P26" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q26" s="24" t="str">
@@ -5471,17 +5477,17 @@
     </row>
     <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
-      <c r="B27" s="147"/>
+      <c r="B27" s="74"/>
       <c r="C27" s="34" t="str">
         <f>IF($G27="", "", _xlfn.XLOOKUP($G27,Data!$C$6:$C$123,Data!$B$6:$B$123,#N/A))</f>
         <v/>
       </c>
       <c r="D27" s="41" t="str">
-        <f>IF(E27= "","",E27/$E$33)</f>
-        <v/>
-      </c>
-      <c r="E27" s="141" t="str">
-        <f>IF(C27="", "", K27/$K$34)</f>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E27" s="68" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F27" s="6" t="str">
@@ -5489,34 +5495,34 @@
         <v/>
       </c>
       <c r="G27" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H27" s="6" t="str">
-        <f>IF($C27="", "", B27/$B$33)</f>
-        <v/>
-      </c>
-      <c r="I27" s="140" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I27" s="67" t="str">
         <f>IF($C27="", "", _xlfn.XLOOKUP($C27,Data!$B$6:$B$123,Data!$G$6:$G$123,#N/A))</f>
         <v/>
       </c>
-      <c r="J27" s="139" t="str">
-        <f t="shared" si="1"/>
+      <c r="J27" s="66" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K27" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L27" s="80"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L27" s="181"/>
       <c r="M27" s="14"/>
       <c r="N27" s="14"/>
       <c r="O27" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P27" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q27" s="24" t="str">
@@ -5526,17 +5532,17 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
-      <c r="B28" s="147"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="34" t="str">
         <f>IF($G28="", "", _xlfn.XLOOKUP($G28,Data!$C$6:$C$123,Data!$B$6:$B$123,#N/A))</f>
         <v/>
       </c>
       <c r="D28" s="41" t="str">
-        <f>IF(E28= "","",E28/$E$33)</f>
-        <v/>
-      </c>
-      <c r="E28" s="141" t="str">
-        <f>IF(C28="", "", K28/$K$34)</f>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E28" s="68" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F28" s="6" t="str">
@@ -5544,34 +5550,34 @@
         <v/>
       </c>
       <c r="G28" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H28" s="6" t="str">
-        <f>IF($C28="", "", B28/$B$33)</f>
-        <v/>
-      </c>
-      <c r="I28" s="140" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I28" s="67" t="str">
         <f>IF($C28="", "", _xlfn.XLOOKUP($C28,Data!$B$6:$B$123,Data!$G$6:$G$123,#N/A))</f>
         <v/>
       </c>
-      <c r="J28" s="139" t="str">
-        <f t="shared" si="1"/>
+      <c r="J28" s="66" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K28" s="37" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L28" s="80"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L28" s="181"/>
       <c r="M28" s="14"/>
       <c r="N28" s="14"/>
       <c r="O28" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P28" s="14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q28" s="24" t="str">
@@ -5587,11 +5593,11 @@
         <v/>
       </c>
       <c r="D29" s="42" t="str">
-        <f>IF(E29= "","",E29/$E$33)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="E29" s="36" t="str">
-        <f>IF(C29="", "", K29/$K$34)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F29" s="7" t="str">
@@ -5599,11 +5605,11 @@
         <v/>
       </c>
       <c r="G29" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H29" s="7" t="str">
-        <f>IF($C29="", "", B29/$B$33)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I29" s="7" t="str">
@@ -5611,22 +5617,22 @@
         <v/>
       </c>
       <c r="J29" s="38" t="str">
-        <f t="shared" ref="J19:J29" si="7">IF(ISBLANK($B29), "",H29*I29)</f>
+        <f t="shared" ref="J29" si="10">IF(ISBLANK($B29), "",H29*I29)</f>
         <v/>
       </c>
       <c r="K29" s="38" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L29" s="81"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L29" s="182"/>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
       <c r="O29" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P29" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q29" s="25" t="str">
@@ -5635,57 +5641,57 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="89" t="s">
+      <c r="B30" s="142" t="s">
         <v>403</v>
       </c>
-      <c r="E30" s="89" t="s">
+      <c r="E30" s="142" t="s">
         <v>394</v>
       </c>
-      <c r="J30" s="89" t="s">
+      <c r="J30" s="142" t="s">
         <v>428</v>
       </c>
-      <c r="K30" s="89" t="s">
+      <c r="K30" s="142" t="s">
         <v>401</v>
       </c>
-      <c r="N30" s="89" t="s">
+      <c r="N30" s="142" t="s">
         <v>419</v>
       </c>
-      <c r="O30" s="135" t="s">
+      <c r="O30" s="62" t="s">
         <v>429</v>
       </c>
-      <c r="P30" s="171"/>
-      <c r="Q30" s="125"/>
+      <c r="P30" s="98"/>
+      <c r="Q30" s="55"/>
     </row>
     <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="90"/>
-      <c r="E31" s="90"/>
+      <c r="B31" s="143"/>
+      <c r="E31" s="143"/>
       <c r="G31" s="50"/>
-      <c r="J31" s="90"/>
-      <c r="K31" s="90"/>
-      <c r="N31" s="90"/>
-      <c r="O31" s="136" t="s">
+      <c r="J31" s="143"/>
+      <c r="K31" s="143"/>
+      <c r="N31" s="143"/>
+      <c r="O31" s="63" t="s">
         <v>430</v>
       </c>
-      <c r="P31" s="137"/>
-      <c r="Q31" s="146">
+      <c r="P31" s="64"/>
+      <c r="Q31" s="73">
         <f>$P$40</f>
         <v>3.4195131166621888E-4</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="90"/>
-      <c r="E32" s="90"/>
-      <c r="J32" s="142">
+      <c r="B32" s="143"/>
+      <c r="E32" s="143"/>
+      <c r="J32" s="69">
         <f>SUM(J18:J29)</f>
         <v>18.015349999999998</v>
       </c>
-      <c r="K32" s="90"/>
-      <c r="N32" s="90"/>
-      <c r="O32" s="136" t="s">
+      <c r="K32" s="143"/>
+      <c r="N32" s="143"/>
+      <c r="O32" s="63" t="s">
         <v>431</v>
       </c>
-      <c r="P32" s="137"/>
-      <c r="Q32" s="127" t="s">
+      <c r="P32" s="64"/>
+      <c r="Q32" s="57" t="s">
         <v>425</v>
       </c>
     </row>
@@ -5694,20 +5700,20 @@
         <f>SUM(B18:B29)</f>
         <v>1</v>
       </c>
-      <c r="E33" s="143">
+      <c r="E33" s="70">
         <f>SUM(E18:E29)</f>
         <v>3</v>
       </c>
-      <c r="K33" s="90"/>
+      <c r="K33" s="143"/>
       <c r="N33" s="49">
         <f>SUM(N18:N29)</f>
         <v>1</v>
       </c>
-      <c r="O33" s="136" t="s">
+      <c r="O33" s="63" t="s">
         <v>426</v>
       </c>
-      <c r="P33" s="137"/>
-      <c r="Q33" s="127" t="str">
+      <c r="P33" s="64"/>
+      <c r="Q33" s="57" t="str">
         <f xml:space="preserve"> _xlfn.CONCAT("NCAT blood with ", ROUND(100*$N$28, 1), "% iodine (", ROUND($P$41, 1), " ", $Q$41, ")")</f>
         <v>NCAT blood with 0% iodine (-1059.7 mg iodine/mL blood-iodine solution)</v>
       </c>
@@ -5718,24 +5724,24 @@
         <v>5.5508219379584639E-2</v>
       </c>
       <c r="N34" s="3"/>
-      <c r="O34" s="136" t="s">
+      <c r="O34" s="63" t="s">
         <v>432</v>
       </c>
-      <c r="P34" s="137"/>
-      <c r="Q34" s="127" t="s">
+      <c r="P34" s="64"/>
+      <c r="Q34" s="57" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N35" s="3"/>
-      <c r="O35" s="138" t="s">
+      <c r="O35" s="65" t="s">
         <v>455</v>
       </c>
-      <c r="P35" s="148"/>
-      <c r="Q35" s="149"/>
-      <c r="R35" s="149"/>
-      <c r="S35" s="150"/>
-      <c r="T35" s="151" t="s">
+      <c r="P35" s="75"/>
+      <c r="Q35" s="76"/>
+      <c r="R35" s="76"/>
+      <c r="S35" s="77"/>
+      <c r="T35" s="78" t="s">
         <v>435</v>
       </c>
     </row>
@@ -5746,113 +5752,113 @@
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
       <c r="O36" s="3"/>
-      <c r="P36" s="145">
+      <c r="P36" s="72">
         <f>J32</f>
         <v>18.015349999999998</v>
       </c>
-      <c r="Q36" s="127" t="s">
+      <c r="Q36" s="57" t="s">
         <v>450</v>
       </c>
       <c r="R36" s="3"/>
-      <c r="S36" s="126" t="s">
+      <c r="S36" s="56" t="s">
         <v>433</v>
       </c>
-      <c r="T36" s="127" t="s">
+      <c r="T36" s="57" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
-      <c r="P37" s="145">
+      <c r="P37" s="72">
         <v>55845.000000000015</v>
       </c>
-      <c r="Q37" s="127" t="s">
+      <c r="Q37" s="57" t="s">
         <v>451</v>
       </c>
-      <c r="S37" s="144">
+      <c r="S37" s="71">
         <v>0.7</v>
       </c>
-      <c r="T37" s="152">
+      <c r="T37" s="79">
         <v>7.0489999999999997E-3</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
-      <c r="P38" s="128">
+      <c r="P38" s="58">
         <f>P36/P37</f>
         <v>3.2259557704360269E-4</v>
       </c>
-      <c r="Q38" s="127" t="s">
+      <c r="Q38" s="57" t="s">
         <v>452</v>
       </c>
-      <c r="S38" s="144">
+      <c r="S38" s="71">
         <v>0.8</v>
       </c>
-      <c r="T38" s="152">
+      <c r="T38" s="79">
         <v>8.0649999999999993E-3</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="O39" s="53"/>
-      <c r="P39" s="126">
+      <c r="P39" s="56">
         <v>1.06</v>
       </c>
-      <c r="Q39" s="127" t="s">
+      <c r="Q39" s="57" t="s">
         <v>424</v>
       </c>
-      <c r="S39" s="144">
+      <c r="S39" s="71">
         <v>0.9</v>
       </c>
-      <c r="T39" s="152">
+      <c r="T39" s="79">
         <v>9.0819999999999998E-3</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="O40" s="3"/>
-      <c r="P40" s="128">
+      <c r="P40" s="58">
         <f>P38*P39</f>
         <v>3.4195131166621888E-4</v>
       </c>
-      <c r="Q40" s="127" t="s">
+      <c r="Q40" s="57" t="s">
         <v>443</v>
       </c>
-      <c r="S40" s="144">
+      <c r="S40" s="71">
         <v>1</v>
       </c>
-      <c r="T40" s="152">
+      <c r="T40" s="79">
         <v>1.0101000000000001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P41" s="134">
+      <c r="P41" s="61">
         <f>1000*(P40-P39)</f>
         <v>-1059.6580486883338</v>
       </c>
-      <c r="Q41" s="129" t="s">
+      <c r="Q41" s="59" t="s">
         <v>441</v>
       </c>
-      <c r="S41" s="144">
+      <c r="S41" s="71">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T41" s="152">
+      <c r="T41" s="79">
         <v>1.1122E-2</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="S42" s="144">
+      <c r="S42" s="71">
         <v>2</v>
       </c>
-      <c r="T42" s="152">
+      <c r="T42" s="79">
         <v>2.0407999999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S43" s="134">
+      <c r="S43" s="61">
         <v>3</v>
       </c>
-      <c r="T43" s="153">
+      <c r="T43" s="80">
         <v>3.0928000000000001E-2</v>
       </c>
     </row>
@@ -5921,17 +5927,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="37">
-    <mergeCell ref="J1:P1"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A3:P3"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="E12:E17"/>
-    <mergeCell ref="D12:D17"/>
-    <mergeCell ref="G7:P7"/>
-    <mergeCell ref="A10:P10"/>
-    <mergeCell ref="A11:P11"/>
-    <mergeCell ref="F9:P9"/>
+    <mergeCell ref="F12:F17"/>
+    <mergeCell ref="G12:G17"/>
+    <mergeCell ref="I12:I17"/>
+    <mergeCell ref="K12:K17"/>
+    <mergeCell ref="N30:N32"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A4:P4"/>
@@ -5948,16 +5948,22 @@
     <mergeCell ref="N14:N17"/>
     <mergeCell ref="O14:O17"/>
     <mergeCell ref="J30:J31"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A3:P3"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="E12:E17"/>
+    <mergeCell ref="D12:D17"/>
+    <mergeCell ref="G7:P7"/>
+    <mergeCell ref="A10:P10"/>
+    <mergeCell ref="A11:P11"/>
+    <mergeCell ref="F9:P9"/>
     <mergeCell ref="L5:P5"/>
     <mergeCell ref="D6:P6"/>
     <mergeCell ref="F8:P8"/>
     <mergeCell ref="L12:L29"/>
     <mergeCell ref="P14:P17"/>
-    <mergeCell ref="F12:F17"/>
-    <mergeCell ref="G12:G17"/>
-    <mergeCell ref="I12:I17"/>
-    <mergeCell ref="K12:K17"/>
-    <mergeCell ref="N30:N32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5981,102 +5987,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="206" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="I1" s="120" t="s">
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="206"/>
+      <c r="G1" s="206"/>
+      <c r="I1" s="204" t="s">
         <v>374</v>
       </c>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="P1" s="119" t="s">
+      <c r="J1" s="204"/>
+      <c r="K1" s="204"/>
+      <c r="L1" s="204"/>
+      <c r="M1" s="204"/>
+      <c r="N1" s="204"/>
+      <c r="P1" s="203" t="s">
         <v>373</v>
       </c>
-      <c r="Q1" s="119"/>
-      <c r="S1" s="120" t="s">
+      <c r="Q1" s="203"/>
+      <c r="S1" s="204" t="s">
         <v>376</v>
       </c>
-      <c r="T1" s="121"/>
-      <c r="U1" s="121"/>
-      <c r="V1" s="121"/>
+      <c r="T1" s="205"/>
+      <c r="U1" s="205"/>
+      <c r="V1" s="205"/>
     </row>
     <row r="2" spans="1:26" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="207" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="P2" s="119"/>
-      <c r="Q2" s="119"/>
-      <c r="S2" s="121"/>
-      <c r="T2" s="121"/>
-      <c r="U2" s="121"/>
-      <c r="V2" s="121"/>
+      <c r="B2" s="207"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="I2" s="204"/>
+      <c r="J2" s="204"/>
+      <c r="K2" s="204"/>
+      <c r="L2" s="204"/>
+      <c r="M2" s="204"/>
+      <c r="N2" s="204"/>
+      <c r="P2" s="203"/>
+      <c r="Q2" s="203"/>
+      <c r="S2" s="205"/>
+      <c r="T2" s="205"/>
+      <c r="U2" s="205"/>
+      <c r="V2" s="205"/>
     </row>
     <row r="3" spans="1:26" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="207" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="120"/>
-      <c r="P3" s="119"/>
-      <c r="Q3" s="119"/>
-      <c r="S3" s="121"/>
-      <c r="T3" s="121"/>
-      <c r="U3" s="121"/>
-      <c r="V3" s="121"/>
+      <c r="B3" s="207"/>
+      <c r="C3" s="207"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="I3" s="204"/>
+      <c r="J3" s="204"/>
+      <c r="K3" s="204"/>
+      <c r="L3" s="204"/>
+      <c r="M3" s="204"/>
+      <c r="N3" s="204"/>
+      <c r="P3" s="203"/>
+      <c r="Q3" s="203"/>
+      <c r="S3" s="205"/>
+      <c r="T3" s="205"/>
+      <c r="U3" s="205"/>
+      <c r="V3" s="205"/>
     </row>
     <row r="4" spans="1:26" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="124" t="s">
+      <c r="A4" s="208" t="s">
         <v>250</v>
       </c>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="120"/>
-      <c r="P4" s="119"/>
-      <c r="Q4" s="119"/>
-      <c r="S4" s="121"/>
-      <c r="T4" s="121"/>
-      <c r="U4" s="121"/>
-      <c r="V4" s="121"/>
+      <c r="B4" s="208"/>
+      <c r="C4" s="208"/>
+      <c r="D4" s="208"/>
+      <c r="E4" s="208"/>
+      <c r="F4" s="208"/>
+      <c r="G4" s="208"/>
+      <c r="I4" s="204"/>
+      <c r="J4" s="204"/>
+      <c r="K4" s="204"/>
+      <c r="L4" s="204"/>
+      <c r="M4" s="204"/>
+      <c r="N4" s="204"/>
+      <c r="P4" s="203"/>
+      <c r="Q4" s="203"/>
+      <c r="S4" s="205"/>
+      <c r="T4" s="205"/>
+      <c r="U4" s="205"/>
+      <c r="V4" s="205"/>
     </row>
     <row r="5" spans="1:26" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">

</xml_diff>